<commit_message>
JPY Contributor: OIS Fixed Leg --> Act/360
</commit_message>
<xml_diff>
--- a/QuantLibXL/Data2/XLS/JPY_MxContributor.xlsx
+++ b/QuantLibXL/Data2/XLS/JPY_MxContributor.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="-15" yWindow="-15" windowWidth="15285" windowHeight="8550" activeTab="1"/>
+    <workbookView xWindow="-15" yWindow="-15" windowWidth="19230" windowHeight="11610" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="General Settings" sheetId="2" r:id="rId1"/>
@@ -28,12 +28,14 @@
     <definedName name="CurveTenor" localSheetId="2">'ON Pricing'!$F$1</definedName>
     <definedName name="EvaluationDate">'General Settings'!$D$5</definedName>
     <definedName name="Fields">Contribution!$H$1:$I$1</definedName>
+    <definedName name="FixDayCounter" localSheetId="2">'ON Pricing'!$P$8</definedName>
     <definedName name="FixedLegBDC" localSheetId="4">'6M Pricing'!$P$24</definedName>
     <definedName name="FixedLegBDC">'3M Pricing'!$P$24</definedName>
     <definedName name="FixedLegDayCounter" localSheetId="3">'3M Pricing'!$Q$24</definedName>
     <definedName name="FixedLegDayCounter" localSheetId="4">'6M Pricing'!$Q$24</definedName>
     <definedName name="FixedLegTenor" localSheetId="3">'3M Pricing'!$O$24</definedName>
     <definedName name="FixedLegTenor" localSheetId="4">'6M Pricing'!$O$24</definedName>
+    <definedName name="ForwardStart" localSheetId="2">'ON Pricing'!$O$8</definedName>
     <definedName name="IborIndex" localSheetId="3">'3M Pricing'!$M$13</definedName>
     <definedName name="IborIndex" localSheetId="4">'6M Pricing'!$M$16</definedName>
     <definedName name="IborIndexFamily">'General Settings'!$D$12</definedName>
@@ -90,7 +92,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="547" uniqueCount="134">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="551" uniqueCount="138">
   <si>
     <t>BID</t>
   </si>
@@ -492,6 +494,18 @@
   </si>
   <si>
     <t>LiborCalendar</t>
+  </si>
+  <si>
+    <t>ForwardStart</t>
+  </si>
+  <si>
+    <t>FixDayCounter</t>
+  </si>
+  <si>
+    <t>0D</t>
+  </si>
+  <si>
+    <t>Actual/360</t>
   </si>
 </sst>
 </file>
@@ -1405,259 +1419,259 @@
 <volTypes xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <volType type="realTimeData">
     <main first="pldatasource.rtgetrtdserver">
-      <tp>
-        <v>0.17499999999999999</v>
+      <tp t="s">
+        <v>#N/A Invalid source.</v>
         <stp/>
         <stp xml:space="preserve">
 JPY6M2x8F=_x0003_BID_x0007_DTSIMI1ÿ_x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000_</stp>
         <tr r="X18" s="7"/>
       </tp>
-      <tp>
-        <v>0.17</v>
+      <tp t="s">
+        <v>#N/A Invalid source.</v>
         <stp/>
         <stp xml:space="preserve">
 JPY6M3x9F=_x0003_BID_x0007_DTSIMI1ÿ_x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000_</stp>
         <tr r="X19" s="7"/>
       </tp>
-      <tp>
-        <v>0.17</v>
+      <tp t="s">
+        <v>#N/A Invalid source.</v>
         <stp/>
         <stp xml:space="preserve">
 JPY6M3x9F=_x0003_ASK_x0007_DTSIMI1ÿ_x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000_</stp>
         <tr r="Y19" s="7"/>
       </tp>
-      <tp>
-        <v>0.17499999999999999</v>
+      <tp t="s">
+        <v>#N/A Invalid source.</v>
         <stp/>
         <stp xml:space="preserve">
 JPY6M2x8F=_x0003_ASK_x0007_DTSIMI1ÿ_x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000_</stp>
         <tr r="Y18" s="7"/>
       </tp>
-      <tp>
-        <v>6.4290683000000001E-2</v>
+      <tp t="s">
+        <v>#N/A Invalid source.</v>
         <stp/>
         <stp xml:space="preserve">	JPYONSND=_x0003_ASK_x0007_DTSIMI1ÿ_x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000_</stp>
         <tr r="K7" s="7"/>
       </tp>
-      <tp>
-        <v>6.3456116000000007E-2</v>
+      <tp t="s">
+        <v>#N/A Invalid source.</v>
         <stp/>
         <stp xml:space="preserve">	JPYONSWD=_x0003_ASK_x0007_DTSIMI1ÿ_x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000_</stp>
         <tr r="K8" s="7"/>
       </tp>
-      <tp>
-        <v>6.4284050999999995E-2</v>
+      <tp t="s">
+        <v>#N/A Invalid source.</v>
         <stp/>
         <stp xml:space="preserve">	JPYONTND=_x0003_ASK_x0007_DTSIMI1ÿ_x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000_</stp>
         <tr r="K6" s="7"/>
       </tp>
-      <tp>
-        <v>6.4280734000000006E-2</v>
+      <tp t="s">
+        <v>#N/A Invalid source.</v>
         <stp/>
         <stp xml:space="preserve">	JPYONOND=_x0003_ASK_x0007_DTSIMI1ÿ_x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000_</stp>
         <tr r="K5" s="7"/>
       </tp>
-      <tp>
-        <v>6.1643836E-2</v>
+      <tp t="s">
+        <v>#N/A Invalid source.</v>
         <stp/>
         <stp xml:space="preserve">	JPYON3MD=_x0003_ASK_x0007_DTSIMI1ÿ_x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000_</stp>
         <tr r="K13" s="7"/>
       </tp>
-      <tp>
-        <v>6.3716391999999997E-2</v>
+      <tp t="s">
+        <v>#N/A Invalid source.</v>
         <stp/>
         <stp xml:space="preserve">	JPYON3WD=_x0003_ASK_x0007_DTSIMI1ÿ_x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000_</stp>
         <tr r="K10" s="7"/>
       </tp>
-      <tp>
-        <v>6.1643836E-2</v>
+      <tp t="s">
+        <v>#N/A Invalid source.</v>
         <stp/>
         <stp xml:space="preserve">	JPYON3YD=_x0003_ASK_x0007_DTSIMI1ÿ_x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000_</stp>
         <tr r="K26" s="7"/>
       </tp>
-      <tp>
-        <v>6.4109588999999995E-2</v>
+      <tp t="s">
+        <v>#N/A Invalid source.</v>
         <stp/>
         <stp xml:space="preserve">	JPYON2MD=_x0003_ASK_x0007_DTSIMI1ÿ_x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000_</stp>
         <tr r="K12" s="7"/>
       </tp>
-      <tp>
-        <v>6.3559539999999998E-2</v>
+      <tp t="s">
+        <v>#N/A Invalid source.</v>
         <stp/>
         <stp xml:space="preserve">	JPYON2WD=_x0003_ASK_x0007_DTSIMI1ÿ_x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000_</stp>
         <tr r="K9" s="7"/>
       </tp>
-      <tp>
-        <v>5.6712328999999999E-2</v>
+      <tp t="s">
+        <v>#N/A Invalid source.</v>
         <stp/>
         <stp xml:space="preserve">	JPYON2YD=_x0003_ASK_x0007_DTSIMI1ÿ_x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000_</stp>
         <tr r="K25" s="7"/>
       </tp>
-      <tp>
-        <v>6.4109588999999995E-2</v>
+      <tp t="s">
+        <v>#N/A Invalid source.</v>
         <stp/>
         <stp xml:space="preserve">	JPYON1MD=_x0003_ASK_x0007_DTSIMI1ÿ_x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000_</stp>
         <tr r="K11" s="7"/>
       </tp>
-      <tp>
-        <v>5.6712328999999999E-2</v>
+      <tp t="s">
+        <v>#N/A Invalid source.</v>
         <stp/>
         <stp xml:space="preserve">	JPYON1YD=_x0003_ASK_x0007_DTSIMI1ÿ_x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000_</stp>
         <tr r="K22" s="7"/>
       </tp>
-      <tp>
-        <v>0.199726027</v>
+      <tp t="s">
+        <v>#N/A Invalid source.</v>
         <stp/>
         <stp xml:space="preserve">	JPYON7YD=_x0003_ASK_x0007_DTSIMI1ÿ_x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000_</stp>
         <tr r="K30" s="7"/>
       </tp>
-      <tp>
-        <v>5.9178082E-2</v>
+      <tp t="s">
+        <v>#N/A Invalid source.</v>
         <stp/>
         <stp xml:space="preserve">	JPYON6MD=_x0003_ASK_x0007_DTSIMI1ÿ_x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000_</stp>
         <tr r="K16" s="7"/>
       </tp>
-      <tp>
-        <v>0.13561643800000001</v>
+      <tp t="s">
+        <v>#N/A Invalid source.</v>
         <stp/>
         <stp xml:space="preserve">	JPYON6YD=_x0003_ASK_x0007_DTSIMI1ÿ_x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000_</stp>
         <tr r="K29" s="7"/>
       </tp>
-      <tp>
-        <v>6.1643836E-2</v>
+      <tp t="s">
+        <v>#N/A Invalid source.</v>
         <stp/>
         <stp xml:space="preserve">	JPYON5MD=_x0003_ASK_x0007_DTSIMI1ÿ_x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000_</stp>
         <tr r="K15" s="7"/>
       </tp>
-      <tp>
-        <v>9.3698630000000005E-2</v>
+      <tp t="s">
+        <v>#N/A Invalid source.</v>
         <stp/>
         <stp xml:space="preserve">	JPYON5YD=_x0003_ASK_x0007_DTSIMI1ÿ_x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000_</stp>
         <tr r="K28" s="7"/>
       </tp>
-      <tp>
-        <v>6.1643836E-2</v>
+      <tp t="s">
+        <v>#N/A Invalid source.</v>
         <stp/>
         <stp xml:space="preserve">	JPYON4MD=_x0003_ASK_x0007_DTSIMI1ÿ_x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000_</stp>
         <tr r="K14" s="7"/>
       </tp>
-      <tp>
-        <v>6.9041095999999996E-2</v>
+      <tp t="s">
+        <v>#N/A Invalid source.</v>
         <stp/>
         <stp xml:space="preserve">	JPYON4YD=_x0003_ASK_x0007_DTSIMI1ÿ_x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000_</stp>
         <tr r="K27" s="7"/>
       </tp>
-      <tp>
-        <v>5.9178082E-2</v>
+      <tp t="s">
+        <v>#N/A Invalid source.</v>
         <stp/>
         <stp xml:space="preserve">	JPYON9MD=_x0003_ASK_x0007_DTSIMI1ÿ_x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000_</stp>
         <tr r="K19" s="7"/>
       </tp>
-      <tp>
-        <v>0.34027397300000001</v>
+      <tp t="s">
+        <v>#N/A Invalid source.</v>
         <stp/>
         <stp xml:space="preserve">	JPYON9YD=_x0003_ASK_x0007_DTSIMI1ÿ_x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000_</stp>
         <tr r="K32" s="7"/>
       </tp>
-      <tp>
-        <v>0.268767123</v>
+      <tp t="s">
+        <v>#N/A Invalid source.</v>
         <stp/>
         <stp xml:space="preserve">	JPYON8YD=_x0003_ASK_x0007_DTSIMI1ÿ_x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000_</stp>
         <tr r="K31" s="7"/>
       </tp>
-      <tp>
-        <v>0.125</v>
+      <tp t="s">
+        <v>#N/A Invalid source.</v>
         <stp/>
         <stp xml:space="preserve">
 JPY3M6x9F=_x0003_BID_x0007_DTSIMI1ÿ_x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000_</stp>
         <tr r="Q19" s="7"/>
       </tp>
-      <tp>
-        <v>0.125</v>
+      <tp t="s">
+        <v>#N/A Invalid source.</v>
         <stp/>
         <stp xml:space="preserve">
 JPY3M5x8F=_x0003_BID_x0007_DTSIMI1ÿ_x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000_</stp>
         <tr r="Q18" s="7"/>
       </tp>
-      <tp>
-        <v>0.125</v>
+      <tp t="s">
+        <v>#N/A Invalid source.</v>
         <stp/>
         <stp xml:space="preserve">
 JPY3M5x8F=_x0003_ASK_x0007_DTSIMI1ÿ_x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000_</stp>
         <tr r="R18" s="7"/>
       </tp>
-      <tp>
-        <v>0.125</v>
+      <tp t="s">
+        <v>#N/A Invalid source.</v>
         <stp/>
         <stp xml:space="preserve">
 JPY3M6x9F=_x0003_ASK_x0007_DTSIMI1ÿ_x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000_</stp>
         <tr r="R19" s="7"/>
       </tp>
-      <tp>
-        <v>0.13</v>
+      <tp t="s">
+        <v>#N/A Invalid source.</v>
         <stp/>
         <stp xml:space="preserve">
 JPY3M3x6F=_x0003_ASK_x0007_DTSIMI1ÿ_x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000_</stp>
         <tr r="R16" s="7"/>
       </tp>
-      <tp>
-        <v>0.13</v>
+      <tp t="s">
+        <v>#N/A Invalid source.</v>
         <stp/>
         <stp xml:space="preserve">
 JPY3M2x5F=_x0003_BID_x0007_DTSIMI1ÿ_x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000_</stp>
         <tr r="Q15" s="7"/>
       </tp>
-      <tp>
-        <v>0.125</v>
+      <tp t="s">
+        <v>#N/A Invalid source.</v>
         <stp/>
         <stp xml:space="preserve">
 JPY3M4x7F=_x0003_ASK_x0007_DTSIMI1ÿ_x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000_</stp>
         <tr r="R17" s="7"/>
       </tp>
-      <tp>
-        <v>0.13</v>
+      <tp t="s">
+        <v>#N/A Invalid source.</v>
         <stp/>
         <stp xml:space="preserve">
 JPY3M1x4F=_x0003_BID_x0007_DTSIMI1ÿ_x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000_</stp>
         <tr r="Q14" s="7"/>
       </tp>
-      <tp>
-        <v>0.13</v>
+      <tp t="s">
+        <v>#N/A Invalid source.</v>
         <stp/>
         <stp xml:space="preserve">
 JPY3M1x4F=_x0003_ASK_x0007_DTSIMI1ÿ_x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000_</stp>
         <tr r="R14" s="7"/>
       </tp>
-      <tp>
-        <v>0.125</v>
+      <tp t="s">
+        <v>#N/A Invalid source.</v>
         <stp/>
         <stp xml:space="preserve">
 JPY3M4x7F=_x0003_BID_x0007_DTSIMI1ÿ_x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000_</stp>
         <tr r="Q17" s="7"/>
       </tp>
-      <tp>
-        <v>0.13</v>
+      <tp t="s">
+        <v>#N/A Invalid source.</v>
         <stp/>
         <stp xml:space="preserve">
 JPY3M2x5F=_x0003_ASK_x0007_DTSIMI1ÿ_x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000_</stp>
         <tr r="R15" s="7"/>
       </tp>
-      <tp>
-        <v>0.13</v>
+      <tp t="s">
+        <v>#N/A Invalid source.</v>
         <stp/>
         <stp xml:space="preserve">
 JPY3M3x6F=_x0003_BID_x0007_DTSIMI1ÿ_x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000_</stp>
         <tr r="Q16" s="7"/>
       </tp>
-      <tp>
-        <v>0.17499999999999999</v>
+      <tp t="s">
+        <v>#N/A Invalid source.</v>
         <stp/>
         <stp xml:space="preserve">
 JPY6M1x7F=_x0003_ASK_x0007_DTSIMI1ÿ_x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000_</stp>
         <tr r="Y17" s="7"/>
       </tp>
-      <tp>
-        <v>0.17499999999999999</v>
+      <tp t="s">
+        <v>#N/A Invalid source.</v>
         <stp/>
         <stp xml:space="preserve">
 JPY6M1x7F=_x0003_BID_x0007_DTSIMI1ÿ_x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000_</stp>
@@ -1665,51 +1679,51 @@
       </tp>
     </main>
     <main first="pldatasource.rtgetrtdserver">
-      <tp>
-        <v>0.11</v>
+      <tp t="s">
+        <v>#N/A Invalid source.</v>
         <stp/>
         <stp>_x000C_JPY3M12x15F=_x0003_BID_x0007_DTSIMI1ÿ_x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000_</stp>
         <tr r="Q23" s="7"/>
       </tp>
     </main>
     <main first="pldatasource.rtgetrtdserver">
-      <tp>
-        <v>1.3093150680000001</v>
+      <tp t="s">
+        <v>#N/A Invalid source.</v>
         <stp/>
         <stp xml:space="preserve">
 JPYON25YD=_x0003_BID_x0007_DTSIMI1ÿ_x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000_</stp>
         <tr r="J37" s="7"/>
       </tp>
-      <tp>
-        <v>1.1441095889999999</v>
+      <tp t="s">
+        <v>#N/A Invalid source.</v>
         <stp/>
         <stp xml:space="preserve">
 JPYON20YD=_x0003_BID_x0007_DTSIMI1ÿ_x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000_</stp>
         <tr r="J36" s="7"/>
       </tp>
-      <tp>
-        <v>1.410410959</v>
+      <tp t="s">
+        <v>#N/A Invalid source.</v>
         <stp/>
         <stp xml:space="preserve">
 JPYON30YD=_x0003_BID_x0007_DTSIMI1ÿ_x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000_</stp>
         <tr r="J38" s="7"/>
       </tp>
-      <tp>
-        <v>0.83342465799999998</v>
+      <tp t="s">
+        <v>#N/A Invalid source.</v>
         <stp/>
         <stp xml:space="preserve">
 JPYON15YD=_x0003_BID_x0007_DTSIMI1ÿ_x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000_</stp>
         <tr r="J35" s="7"/>
       </tp>
-      <tp>
-        <v>0.41424657500000001</v>
+      <tp t="s">
+        <v>#N/A Invalid source.</v>
         <stp/>
         <stp xml:space="preserve">
 JPYON10YD=_x0003_BID_x0007_DTSIMI1ÿ_x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000_</stp>
         <tr r="J33" s="7"/>
       </tp>
-      <tp>
-        <v>0.58191780800000004</v>
+      <tp t="s">
+        <v>#N/A Invalid source.</v>
         <stp/>
         <stp xml:space="preserve">
 JPYON12YD=_x0003_BID_x0007_DTSIMI1ÿ_x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000_</stp>
@@ -1717,175 +1731,177 @@
       </tp>
     </main>
     <main first="pldatasource.rtgetrtdserver">
-      <tp>
-        <v>6.4290683000000001E-2</v>
+      <tp t="s">
+        <v>#N/A Invalid source.</v>
         <stp/>
         <stp xml:space="preserve">	JPYONSND=_x0003_BID_x0007_DTSIMI1ÿ_x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000_</stp>
         <tr r="J7" s="7"/>
       </tp>
-      <tp>
-        <v>6.3456116000000007E-2</v>
+      <tp t="s">
+        <v>#N/A Invalid source.</v>
         <stp/>
         <stp xml:space="preserve">	JPYONSWD=_x0003_BID_x0007_DTSIMI1ÿ_x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000_</stp>
         <tr r="J8" s="7"/>
       </tp>
-      <tp>
-        <v>6.4284050999999995E-2</v>
+      <tp t="s">
+        <v>#N/A Invalid source.</v>
         <stp/>
         <stp xml:space="preserve">	JPYONTND=_x0003_BID_x0007_DTSIMI1ÿ_x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000_</stp>
         <tr r="J6" s="7"/>
       </tp>
-      <tp>
-        <v>6.4280734000000006E-2</v>
+      <tp t="s">
+        <v>#N/A Invalid source.</v>
         <stp/>
         <stp xml:space="preserve">	JPYONOND=_x0003_BID_x0007_DTSIMI1ÿ_x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000_</stp>
         <tr r="J5" s="7"/>
       </tp>
-      <tp>
-        <v>6.1643836E-2</v>
+      <tp t="s">
+        <v>#N/A Invalid source.</v>
         <stp/>
         <stp xml:space="preserve">	JPYON3MD=_x0003_BID_x0007_DTSIMI1ÿ_x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000_</stp>
         <tr r="J13" s="7"/>
       </tp>
-      <tp>
-        <v>6.3716391999999997E-2</v>
+      <tp t="s">
+        <v>#N/A Invalid source.</v>
         <stp/>
         <stp xml:space="preserve">	JPYON3WD=_x0003_BID_x0007_DTSIMI1ÿ_x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000_</stp>
         <tr r="J10" s="7"/>
       </tp>
-      <tp>
-        <v>6.1643836E-2</v>
+      <tp t="s">
+        <v>#N/A Invalid source.</v>
         <stp/>
         <stp xml:space="preserve">	JPYON3YD=_x0003_BID_x0007_DTSIMI1ÿ_x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000_</stp>
         <tr r="J26" s="7"/>
       </tp>
-      <tp>
-        <v>6.4109588999999995E-2</v>
+      <tp t="s">
+        <v>#N/A Invalid source.</v>
         <stp/>
         <stp xml:space="preserve">	JPYON2MD=_x0003_BID_x0007_DTSIMI1ÿ_x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000_</stp>
         <tr r="J12" s="7"/>
       </tp>
-      <tp>
-        <v>6.3559539999999998E-2</v>
+      <tp t="s">
+        <v>#N/A Invalid source.</v>
         <stp/>
         <stp xml:space="preserve">	JPYON2WD=_x0003_BID_x0007_DTSIMI1ÿ_x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000_</stp>
         <tr r="J9" s="7"/>
       </tp>
-      <tp>
-        <v>5.6712328999999999E-2</v>
+      <tp t="s">
+        <v>#N/A Invalid source.</v>
         <stp/>
         <stp xml:space="preserve">	JPYON2YD=_x0003_BID_x0007_DTSIMI1ÿ_x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000_</stp>
         <tr r="J25" s="7"/>
       </tp>
-      <tp>
-        <v>6.4109588999999995E-2</v>
+      <tp t="s">
+        <v>#N/A Invalid source.</v>
         <stp/>
         <stp xml:space="preserve">	JPYON1MD=_x0003_BID_x0007_DTSIMI1ÿ_x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000_</stp>
         <tr r="J11" s="7"/>
       </tp>
-      <tp>
-        <v>5.6712328999999999E-2</v>
+      <tp t="s">
+        <v>#N/A Invalid source.</v>
         <stp/>
         <stp xml:space="preserve">	JPYON1YD=_x0003_BID_x0007_DTSIMI1ÿ_x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000_</stp>
         <tr r="J22" s="7"/>
       </tp>
-      <tp>
-        <v>0.199726027</v>
+      <tp t="s">
+        <v>#N/A Invalid source.</v>
         <stp/>
         <stp xml:space="preserve">	JPYON7YD=_x0003_BID_x0007_DTSIMI1ÿ_x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000_</stp>
         <tr r="J30" s="7"/>
       </tp>
-      <tp>
-        <v>5.9178082E-2</v>
+      <tp t="s">
+        <v>#N/A Invalid source.</v>
         <stp/>
         <stp xml:space="preserve">	JPYON6MD=_x0003_BID_x0007_DTSIMI1ÿ_x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000_</stp>
         <tr r="J16" s="7"/>
       </tp>
-      <tp>
-        <v>0.13561643800000001</v>
+      <tp t="s">
+        <v>#N/A Invalid source.</v>
         <stp/>
         <stp xml:space="preserve">	JPYON6YD=_x0003_BID_x0007_DTSIMI1ÿ_x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000_</stp>
         <tr r="J29" s="7"/>
       </tp>
-      <tp>
-        <v>6.1643836E-2</v>
+      <tp t="s">
+        <v>#N/A Invalid source.</v>
         <stp/>
         <stp xml:space="preserve">	JPYON5MD=_x0003_BID_x0007_DTSIMI1ÿ_x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000_</stp>
         <tr r="J15" s="7"/>
       </tp>
-      <tp>
-        <v>9.3698630000000005E-2</v>
+      <tp t="s">
+        <v>#N/A Invalid source.</v>
         <stp/>
         <stp xml:space="preserve">	JPYON5YD=_x0003_BID_x0007_DTSIMI1ÿ_x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000_</stp>
         <tr r="J28" s="7"/>
       </tp>
-      <tp>
-        <v>6.1643836E-2</v>
+      <tp t="s">
+        <v>#N/A Invalid source.</v>
         <stp/>
         <stp xml:space="preserve">	JPYON4MD=_x0003_BID_x0007_DTSIMI1ÿ_x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000_</stp>
         <tr r="J14" s="7"/>
       </tp>
-      <tp>
-        <v>6.9041095999999996E-2</v>
+      <tp t="s">
+        <v>#N/A Invalid source.</v>
         <stp/>
         <stp xml:space="preserve">	JPYON4YD=_x0003_BID_x0007_DTSIMI1ÿ_x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000_</stp>
         <tr r="J27" s="7"/>
       </tp>
-      <tp>
-        <v>5.9178082E-2</v>
+      <tp t="s">
+        <v>#N/A Invalid source.</v>
         <stp/>
         <stp xml:space="preserve">	JPYON9MD=_x0003_BID_x0007_DTSIMI1ÿ_x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000_</stp>
         <tr r="J19" s="7"/>
       </tp>
-      <tp>
-        <v>0.34027397300000001</v>
+      <tp t="s">
+        <v>#N/A Invalid source.</v>
         <stp/>
         <stp xml:space="preserve">	JPYON9YD=_x0003_BID_x0007_DTSIMI1ÿ_x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000_</stp>
         <tr r="J32" s="7"/>
       </tp>
-      <tp>
-        <v>0.268767123</v>
+      <tp t="s">
+        <v>#N/A Invalid source.</v>
         <stp/>
         <stp xml:space="preserve">	JPYON8YD=_x0003_BID_x0007_DTSIMI1ÿ_x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000_</stp>
         <tr r="J31" s="7"/>
       </tp>
-      <tp>
-        <v>0.83342465799999998</v>
+    </main>
+    <main first="pldatasource.rtgetrtdserver">
+      <tp t="s">
+        <v>#N/A Invalid source.</v>
         <stp/>
         <stp xml:space="preserve">
 JPYON15YD=_x0003_ASK_x0007_DTSIMI1ÿ_x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000_</stp>
         <tr r="K35" s="7"/>
       </tp>
-      <tp>
-        <v>0.41424657500000001</v>
+      <tp t="s">
+        <v>#N/A Invalid source.</v>
         <stp/>
         <stp xml:space="preserve">
 JPYON10YD=_x0003_ASK_x0007_DTSIMI1ÿ_x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000_</stp>
         <tr r="K33" s="7"/>
       </tp>
-      <tp>
-        <v>0.58191780800000004</v>
+      <tp t="s">
+        <v>#N/A Invalid source.</v>
         <stp/>
         <stp xml:space="preserve">
 JPYON12YD=_x0003_ASK_x0007_DTSIMI1ÿ_x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000_</stp>
         <tr r="K34" s="7"/>
       </tp>
-      <tp>
-        <v>1.410410959</v>
+      <tp t="s">
+        <v>#N/A Invalid source.</v>
         <stp/>
         <stp xml:space="preserve">
 JPYON30YD=_x0003_ASK_x0007_DTSIMI1ÿ_x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000_</stp>
         <tr r="K38" s="7"/>
       </tp>
-      <tp>
-        <v>1.3093150680000001</v>
+      <tp t="s">
+        <v>#N/A Invalid source.</v>
         <stp/>
         <stp xml:space="preserve">
 JPYON25YD=_x0003_ASK_x0007_DTSIMI1ÿ_x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000_</stp>
         <tr r="K37" s="7"/>
       </tp>
-      <tp>
-        <v>1.1441095889999999</v>
+      <tp t="s">
+        <v>#N/A Invalid source.</v>
         <stp/>
         <stp xml:space="preserve">
 JPYON20YD=_x0003_ASK_x0007_DTSIMI1ÿ_x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000_</stp>
@@ -1893,696 +1909,692 @@
       </tp>
     </main>
     <main first="pldatasource.rtgetrtdserver">
-      <tp>
-        <v>0.11</v>
+      <tp t="s">
+        <v>#N/A Invalid source.</v>
         <stp/>
         <stp>_x000C_JPY3M12x15F=_x0003_ASK_x0007_DTSIMI1ÿ_x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000_</stp>
         <tr r="R23" s="7"/>
       </tp>
-    </main>
-    <main first="pldatasource.rtgetrtdserver">
-      <tp>
-        <v>0.23113118199999999</v>
+      <tp t="s">
+        <v>#N/A Invalid source.</v>
         <stp/>
         <stp xml:space="preserve">	JPY6MSND=_x0003_BID_x0007_DTSIMI1ÿ_x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000_</stp>
         <tr r="X7" s="7"/>
       </tp>
-      <tp>
-        <v>0.23094794699999999</v>
+      <tp t="s">
+        <v>#N/A Invalid source.</v>
         <stp/>
         <stp xml:space="preserve">	JPY6MSWD=_x0003_BID_x0007_DTSIMI1ÿ_x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000_</stp>
         <tr r="X8" s="7"/>
       </tp>
-      <tp>
-        <v>0.231152212</v>
+      <tp t="s">
+        <v>#N/A Invalid source.</v>
         <stp/>
         <stp xml:space="preserve">	JPY6MTND=_x0003_BID_x0007_DTSIMI1ÿ_x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000_</stp>
         <tr r="X6" s="7"/>
       </tp>
-      <tp>
-        <v>0.231174873</v>
+      <tp t="s">
+        <v>#N/A Invalid source.</v>
         <stp/>
         <stp xml:space="preserve">	JPY6MOND=_x0003_BID_x0007_DTSIMI1ÿ_x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000_</stp>
         <tr r="X5" s="7"/>
       </tp>
-      <tp>
-        <v>0.2064</v>
+      <tp t="s">
+        <v>#N/A Invalid source.</v>
         <stp/>
         <stp xml:space="preserve">	JPY6M3MD=_x0003_BID_x0007_DTSIMI1ÿ_x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000_</stp>
         <tr r="X13" s="7"/>
       </tp>
-      <tp>
-        <v>0.229425409</v>
+      <tp t="s">
+        <v>#N/A Invalid source.</v>
         <stp/>
         <stp xml:space="preserve">	JPY6M3WD=_x0003_BID_x0007_DTSIMI1ÿ_x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000_</stp>
         <tr r="X10" s="7"/>
       </tp>
-      <tp>
-        <v>0.21729999999999999</v>
+      <tp t="s">
+        <v>#N/A Invalid source.</v>
         <stp/>
         <stp xml:space="preserve">	JPY6M2MD=_x0003_BID_x0007_DTSIMI1ÿ_x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000_</stp>
         <tr r="X12" s="7"/>
       </tp>
-      <tp>
-        <v>0.230378317</v>
+      <tp t="s">
+        <v>#N/A Invalid source.</v>
         <stp/>
         <stp xml:space="preserve">	JPY6M2WD=_x0003_BID_x0007_DTSIMI1ÿ_x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000_</stp>
         <tr r="X9" s="7"/>
       </tp>
-      <tp>
-        <v>0.22689999999999999</v>
+      <tp t="s">
+        <v>#N/A Invalid source.</v>
         <stp/>
         <stp xml:space="preserve">	JPY6M1MD=_x0003_BID_x0007_DTSIMI1ÿ_x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000_</stp>
         <tr r="X11" s="7"/>
       </tp>
-      <tp>
-        <v>0.1865</v>
+      <tp t="s">
+        <v>#N/A Invalid source.</v>
         <stp/>
         <stp xml:space="preserve">	JPY6M6MD=_x0003_BID_x0007_DTSIMI1ÿ_x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000_</stp>
         <tr r="X16" s="7"/>
       </tp>
-      <tp>
-        <v>0.19339999999999999</v>
+      <tp t="s">
+        <v>#N/A Invalid source.</v>
         <stp/>
         <stp xml:space="preserve">	JPY6M5MD=_x0003_BID_x0007_DTSIMI1ÿ_x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000_</stp>
         <tr r="X15" s="7"/>
       </tp>
-      <tp>
-        <v>0.19889999999999999</v>
+      <tp t="s">
+        <v>#N/A Invalid source.</v>
         <stp/>
         <stp xml:space="preserve">	JPY6M4MD=_x0003_BID_x0007_DTSIMI1ÿ_x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000_</stp>
         <tr r="X14" s="7"/>
       </tp>
-      <tp>
-        <v>0.47824467599999998</v>
+      <tp t="s">
+        <v>#N/A Invalid source.</v>
         <stp/>
         <stp>_x0008_JPY3M9Y=_x0003_ASK_x0007_DTSIMI1ÿ_x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000_</stp>
         <tr r="R32" s="7"/>
       </tp>
-      <tp>
-        <v>0.39343523699999999</v>
+      <tp t="s">
+        <v>#N/A Invalid source.</v>
         <stp/>
         <stp>_x0008_JPY3M8Y=_x0003_ASK_x0007_DTSIMI1ÿ_x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000_</stp>
         <tr r="R31" s="7"/>
       </tp>
-      <tp>
-        <v>0.11672265499999999</v>
+      <tp t="s">
+        <v>#N/A Invalid source.</v>
         <stp/>
         <stp>_x0008_JPY3M3Y=_x0003_ASK_x0007_DTSIMI1ÿ_x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000_</stp>
         <tr r="R26" s="7"/>
       </tp>
-      <tp>
-        <v>0.11932841800000001</v>
+      <tp t="s">
+        <v>#N/A Invalid source.</v>
         <stp/>
         <stp>_x0008_JPY3M2Y=_x0003_ASK_x0007_DTSIMI1ÿ_x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000_</stp>
         <tr r="R25" s="7"/>
       </tp>
-      <tp>
-        <v>0.17392729700000001</v>
+      <tp t="s">
+        <v>#N/A Invalid source.</v>
         <stp/>
         <stp>_x0008_JPY3M5Y=_x0003_ASK_x0007_DTSIMI1ÿ_x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000_</stp>
         <tr r="R28" s="7"/>
       </tp>
-      <tp>
-        <v>0.13661405600000001</v>
+      <tp t="s">
+        <v>#N/A Invalid source.</v>
         <stp/>
         <stp>_x0008_JPY3M4Y=_x0003_ASK_x0007_DTSIMI1ÿ_x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000_</stp>
         <tr r="R27" s="7"/>
       </tp>
-      <tp>
-        <v>0.31114283999999998</v>
+      <tp t="s">
+        <v>#N/A Invalid source.</v>
         <stp/>
         <stp>_x0008_JPY3M7Y=_x0003_ASK_x0007_DTSIMI1ÿ_x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000_</stp>
         <tr r="R30" s="7"/>
       </tp>
-      <tp>
-        <v>0.23629592499999999</v>
+      <tp t="s">
+        <v>#N/A Invalid source.</v>
         <stp/>
         <stp>_x0008_JPY3M6Y=_x0003_ASK_x0007_DTSIMI1ÿ_x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000_</stp>
         <tr r="R29" s="7"/>
       </tp>
     </main>
     <main first="pldatasource.rtgetrtdserver">
-      <tp>
-        <v>1.582429437</v>
+      <tp t="s">
+        <v>#N/A Invalid source.</v>
         <stp/>
         <stp xml:space="preserve">	JPY3M30Y=_x0003_ASK_x0007_DTSIMI1ÿ_x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000_</stp>
         <tr r="R38" s="7"/>
       </tp>
-      <tp>
-        <v>1.4851867670000001</v>
+      <tp t="s">
+        <v>#N/A Invalid source.</v>
         <stp/>
         <stp xml:space="preserve">	JPY3M25Y=_x0003_ASK_x0007_DTSIMI1ÿ_x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000_</stp>
         <tr r="R37" s="7"/>
       </tp>
-      <tp>
-        <v>1.313468232</v>
+      <tp t="s">
+        <v>#N/A Invalid source.</v>
         <stp/>
         <stp xml:space="preserve">	JPY3M20Y=_x0003_ASK_x0007_DTSIMI1ÿ_x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000_</stp>
         <tr r="R36" s="7"/>
       </tp>
-      <tp>
-        <v>0.99441074200000001</v>
+      <tp t="s">
+        <v>#N/A Invalid source.</v>
         <stp/>
         <stp xml:space="preserve">	JPY3M15Y=_x0003_ASK_x0007_DTSIMI1ÿ_x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000_</stp>
         <tr r="R35" s="7"/>
       </tp>
-      <tp>
-        <v>0.74009947700000001</v>
+      <tp t="s">
+        <v>#N/A Invalid source.</v>
         <stp/>
         <stp xml:space="preserve">	JPY3M12Y=_x0003_ASK_x0007_DTSIMI1ÿ_x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000_</stp>
         <tr r="R34" s="7"/>
       </tp>
-      <tp>
-        <v>0.56303451500000001</v>
+      <tp t="s">
+        <v>#N/A Invalid source.</v>
         <stp/>
         <stp xml:space="preserve">	JPY3M10Y=_x0003_ASK_x0007_DTSIMI1ÿ_x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000_</stp>
         <tr r="R33" s="7"/>
       </tp>
     </main>
     <main first="pldatasource.rtgetrtdserver">
-      <tp>
-        <v>0.138393131</v>
+      <tp t="s">
+        <v>#N/A Invalid source.</v>
         <stp/>
         <stp xml:space="preserve">	JPY3MSND=_x0003_BID_x0007_DTSIMI1ÿ_x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000_</stp>
         <tr r="Q7" s="7"/>
       </tp>
-      <tp>
-        <v>0.138377009</v>
+      <tp t="s">
+        <v>#N/A Invalid source.</v>
         <stp/>
         <stp xml:space="preserve">	JPY3MSWD=_x0003_BID_x0007_DTSIMI1ÿ_x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000_</stp>
         <tr r="Q8" s="7"/>
       </tp>
-      <tp>
-        <v>0.13840192900000001</v>
+      <tp t="s">
+        <v>#N/A Invalid source.</v>
         <stp/>
         <stp xml:space="preserve">	JPY3MTND=_x0003_BID_x0007_DTSIMI1ÿ_x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000_</stp>
         <tr r="Q6" s="7"/>
       </tp>
-      <tp>
-        <v>0.13840522499999999</v>
+      <tp t="s">
+        <v>#N/A Invalid source.</v>
         <stp/>
         <stp xml:space="preserve">	JPY3MOND=_x0003_BID_x0007_DTSIMI1ÿ_x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000_</stp>
         <tr r="Q5" s="7"/>
       </tp>
-      <tp>
-        <v>0.13250000000000001</v>
+      <tp t="s">
+        <v>#N/A Invalid source.</v>
         <stp/>
         <stp xml:space="preserve">	JPY3M3MD=_x0003_BID_x0007_DTSIMI1ÿ_x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000_</stp>
         <tr r="Q13" s="7"/>
       </tp>
-      <tp>
-        <v>0.13823602900000001</v>
+      <tp t="s">
+        <v>#N/A Invalid source.</v>
         <stp/>
         <stp xml:space="preserve">	JPY3M3WD=_x0003_BID_x0007_DTSIMI1ÿ_x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000_</stp>
         <tr r="Q10" s="7"/>
       </tp>
-      <tp>
-        <v>0.1361</v>
+      <tp t="s">
+        <v>#N/A Invalid source.</v>
         <stp/>
         <stp xml:space="preserve">	JPY3M2MD=_x0003_BID_x0007_DTSIMI1ÿ_x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000_</stp>
         <tr r="Q12" s="7"/>
       </tp>
-      <tp>
-        <v>0.13832460899999999</v>
+      <tp t="s">
+        <v>#N/A Invalid source.</v>
         <stp/>
         <stp xml:space="preserve">	JPY3M2WD=_x0003_BID_x0007_DTSIMI1ÿ_x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000_</stp>
         <tr r="Q9" s="7"/>
       </tp>
-      <tp>
-        <v>0.13800000000000001</v>
+      <tp t="s">
+        <v>#N/A Invalid source.</v>
         <stp/>
         <stp xml:space="preserve">	JPY3M1MD=_x0003_BID_x0007_DTSIMI1ÿ_x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000_</stp>
         <tr r="Q11" s="7"/>
       </tp>
-      <tp>
-        <v>0.58750000000000002</v>
+      <tp t="s">
+        <v>#N/A Invalid source.</v>
         <stp/>
         <stp>_x0008_JPY6M9Y=_x0003_ASK_x0007_DTSIMI1ÿ_x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000_</stp>
         <tr r="Y32" s="7"/>
       </tp>
-      <tp>
-        <v>0.495</v>
+      <tp t="s">
+        <v>#N/A Invalid source.</v>
         <stp/>
         <stp>_x0008_JPY6M8Y=_x0003_ASK_x0007_DTSIMI1ÿ_x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000_</stp>
         <tr r="Y31" s="7"/>
       </tp>
-      <tp>
-        <v>0.17249999999999999</v>
+      <tp t="s">
+        <v>#N/A Invalid source.</v>
         <stp/>
         <stp>_x0008_JPY6M3Y=_x0003_ASK_x0007_DTSIMI1ÿ_x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000_</stp>
         <tr r="Y26" s="7"/>
       </tp>
-      <tp>
-        <v>0.16750000000000001</v>
+      <tp t="s">
+        <v>#N/A Invalid source.</v>
         <stp/>
         <stp>_x0008_JPY6M2Y=_x0003_ASK_x0007_DTSIMI1ÿ_x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000_</stp>
         <tr r="Y25" s="7"/>
       </tp>
-      <tp>
-        <v>0.25</v>
+      <tp t="s">
+        <v>#N/A Invalid source.</v>
         <stp/>
         <stp>_x0008_JPY6M5Y=_x0003_ASK_x0007_DTSIMI1ÿ_x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000_</stp>
         <tr r="Y28" s="7"/>
       </tp>
-      <tp>
-        <v>0.2</v>
+      <tp t="s">
+        <v>#N/A Invalid source.</v>
         <stp/>
         <stp>_x0008_JPY6M4Y=_x0003_ASK_x0007_DTSIMI1ÿ_x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000_</stp>
         <tr r="Y27" s="7"/>
       </tp>
-      <tp>
-        <v>0.40250000000000002</v>
+      <tp t="s">
+        <v>#N/A Invalid source.</v>
         <stp/>
         <stp>_x0008_JPY6M7Y=_x0003_ASK_x0007_DTSIMI1ÿ_x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000_</stp>
         <tr r="Y30" s="7"/>
       </tp>
-      <tp>
-        <v>0.32</v>
+      <tp t="s">
+        <v>#N/A Invalid source.</v>
         <stp/>
         <stp>_x0008_JPY6M6Y=_x0003_ASK_x0007_DTSIMI1ÿ_x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000_</stp>
         <tr r="Y29" s="7"/>
       </tp>
     </main>
     <main first="pldatasource.rtgetrtdserver">
-      <tp>
-        <v>1.73</v>
+      <tp t="s">
+        <v>#N/A Invalid source.</v>
         <stp/>
         <stp xml:space="preserve">	JPY6M30Y=_x0003_ASK_x0007_DTSIMI1ÿ_x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000_</stp>
         <tr r="Y38" s="7"/>
       </tp>
-      <tp>
-        <v>1.6274999999999999</v>
+      <tp t="s">
+        <v>#N/A Invalid source.</v>
         <stp/>
         <stp xml:space="preserve">	JPY6M25Y=_x0003_ASK_x0007_DTSIMI1ÿ_x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000_</stp>
         <tr r="Y37" s="7"/>
       </tp>
-      <tp>
-        <v>1.4550000000000001</v>
+      <tp t="s">
+        <v>#N/A Invalid source.</v>
         <stp/>
         <stp xml:space="preserve">	JPY6M20Y=_x0003_ASK_x0007_DTSIMI1ÿ_x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000_</stp>
         <tr r="Y36" s="7"/>
       </tp>
-      <tp>
-        <v>1.1325000000000001</v>
+      <tp t="s">
+        <v>#N/A Invalid source.</v>
         <stp/>
         <stp xml:space="preserve">	JPY6M15Y=_x0003_ASK_x0007_DTSIMI1ÿ_x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000_</stp>
         <tr r="Y35" s="7"/>
       </tp>
-      <tp>
-        <v>0.86750000000000005</v>
+      <tp t="s">
+        <v>#N/A Invalid source.</v>
         <stp/>
         <stp xml:space="preserve">	JPY6M12Y=_x0003_ASK_x0007_DTSIMI1ÿ_x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000_</stp>
         <tr r="Y34" s="7"/>
       </tp>
-      <tp>
-        <v>0.68</v>
+      <tp t="s">
+        <v>#N/A Invalid source.</v>
         <stp/>
         <stp xml:space="preserve">	JPY6M10Y=_x0003_ASK_x0007_DTSIMI1ÿ_x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000_</stp>
         <tr r="Y33" s="7"/>
       </tp>
     </main>
     <main first="pldatasource.rtgetrtdserver">
-      <tp>
-        <v>0.17</v>
+      <tp t="s">
+        <v>#N/A Invalid source.</v>
         <stp/>
         <stp xml:space="preserve">	JPY6M18M=_x0003_BID_x0007_DTSIMI1ÿ_x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000_</stp>
         <tr r="X24" s="7"/>
       </tp>
-    </main>
-    <main first="pldatasource.rtgetrtdserver">
-      <tp>
-        <v>0.495</v>
+      <tp t="s">
+        <v>#N/A Invalid source.</v>
         <stp/>
         <stp>_x0008_JPY6M8Y=_x0003_BID_x0007_DTSIMI1ÿ_x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000_</stp>
         <tr r="X31" s="7"/>
       </tp>
-      <tp>
-        <v>0.58750000000000002</v>
+      <tp t="s">
+        <v>#N/A Invalid source.</v>
         <stp/>
         <stp>_x0008_JPY6M9Y=_x0003_BID_x0007_DTSIMI1ÿ_x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000_</stp>
         <tr r="X32" s="7"/>
       </tp>
-      <tp>
-        <v>0.16750000000000001</v>
+      <tp t="s">
+        <v>#N/A Invalid source.</v>
         <stp/>
         <stp>_x0008_JPY6M2Y=_x0003_BID_x0007_DTSIMI1ÿ_x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000_</stp>
         <tr r="X25" s="7"/>
       </tp>
-      <tp>
-        <v>0.17249999999999999</v>
+      <tp t="s">
+        <v>#N/A Invalid source.</v>
         <stp/>
         <stp>_x0008_JPY6M3Y=_x0003_BID_x0007_DTSIMI1ÿ_x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000_</stp>
         <tr r="X26" s="7"/>
       </tp>
-      <tp>
-        <v>0.32</v>
+      <tp t="s">
+        <v>#N/A Invalid source.</v>
         <stp/>
         <stp>_x0008_JPY6M6Y=_x0003_BID_x0007_DTSIMI1ÿ_x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000_</stp>
         <tr r="X29" s="7"/>
       </tp>
-      <tp>
-        <v>0.40250000000000002</v>
+      <tp t="s">
+        <v>#N/A Invalid source.</v>
         <stp/>
         <stp>_x0008_JPY6M7Y=_x0003_BID_x0007_DTSIMI1ÿ_x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000_</stp>
         <tr r="X30" s="7"/>
       </tp>
-      <tp>
-        <v>0.2</v>
+      <tp t="s">
+        <v>#N/A Invalid source.</v>
         <stp/>
         <stp>_x0008_JPY6M4Y=_x0003_BID_x0007_DTSIMI1ÿ_x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000_</stp>
         <tr r="X27" s="7"/>
       </tp>
-      <tp>
-        <v>0.25</v>
+      <tp t="s">
+        <v>#N/A Invalid source.</v>
         <stp/>
         <stp>_x0008_JPY6M5Y=_x0003_BID_x0007_DTSIMI1ÿ_x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000_</stp>
         <tr r="X28" s="7"/>
       </tp>
     </main>
     <main first="pldatasource.rtgetrtdserver">
-      <tp>
-        <v>0.121242482</v>
+      <tp t="s">
+        <v>#N/A Invalid source.</v>
         <stp/>
         <stp xml:space="preserve">	JPY3M18M=_x0003_BID_x0007_DTSIMI1ÿ_x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000_</stp>
         <tr r="Q24" s="7"/>
       </tp>
     </main>
     <main first="pldatasource.rtgetrtdserver">
-      <tp>
-        <v>0.39343523699999999</v>
+      <tp t="s">
+        <v>#N/A Invalid source.</v>
         <stp/>
         <stp>_x0008_JPY3M8Y=_x0003_BID_x0007_DTSIMI1ÿ_x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000_</stp>
         <tr r="Q31" s="7"/>
       </tp>
-      <tp>
-        <v>0.47824467599999998</v>
+      <tp t="s">
+        <v>#N/A Invalid source.</v>
         <stp/>
         <stp>_x0008_JPY3M9Y=_x0003_BID_x0007_DTSIMI1ÿ_x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000_</stp>
         <tr r="Q32" s="7"/>
       </tp>
-      <tp>
-        <v>0.11932841800000001</v>
+      <tp t="s">
+        <v>#N/A Invalid source.</v>
         <stp/>
         <stp>_x0008_JPY3M2Y=_x0003_BID_x0007_DTSIMI1ÿ_x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000_</stp>
         <tr r="Q25" s="7"/>
       </tp>
-      <tp>
-        <v>0.11672265499999999</v>
+      <tp t="s">
+        <v>#N/A Invalid source.</v>
         <stp/>
         <stp>_x0008_JPY3M3Y=_x0003_BID_x0007_DTSIMI1ÿ_x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000_</stp>
         <tr r="Q26" s="7"/>
       </tp>
-      <tp>
-        <v>0.23629592499999999</v>
+      <tp t="s">
+        <v>#N/A Invalid source.</v>
         <stp/>
         <stp>_x0008_JPY3M6Y=_x0003_BID_x0007_DTSIMI1ÿ_x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000_</stp>
         <tr r="Q29" s="7"/>
       </tp>
-      <tp>
-        <v>0.31114283999999998</v>
+      <tp t="s">
+        <v>#N/A Invalid source.</v>
         <stp/>
         <stp>_x0008_JPY3M7Y=_x0003_BID_x0007_DTSIMI1ÿ_x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000_</stp>
         <tr r="Q30" s="7"/>
       </tp>
-      <tp>
-        <v>0.13661405600000001</v>
+      <tp t="s">
+        <v>#N/A Invalid source.</v>
         <stp/>
         <stp>_x0008_JPY3M4Y=_x0003_BID_x0007_DTSIMI1ÿ_x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000_</stp>
         <tr r="Q27" s="7"/>
       </tp>
-      <tp>
-        <v>0.17392729700000001</v>
+      <tp t="s">
+        <v>#N/A Invalid source.</v>
         <stp/>
         <stp>_x0008_JPY3M5Y=_x0003_BID_x0007_DTSIMI1ÿ_x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000_</stp>
         <tr r="Q28" s="7"/>
       </tp>
-      <tp>
-        <v>0.17</v>
+      <tp t="s">
+        <v>#N/A Invalid source.</v>
         <stp/>
         <stp xml:space="preserve">	JPY6M18M=_x0003_ASK_x0007_DTSIMI1ÿ_x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000_</stp>
         <tr r="Y24" s="7"/>
       </tp>
-      <tp>
-        <v>0.121242482</v>
+      <tp t="s">
+        <v>#N/A Invalid source.</v>
         <stp/>
         <stp xml:space="preserve">	JPY3M18M=_x0003_ASK_x0007_DTSIMI1ÿ_x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000_</stp>
         <tr r="R24" s="7"/>
       </tp>
-      <tp>
-        <v>1.582429437</v>
+      <tp t="s">
+        <v>#N/A Invalid source.</v>
         <stp/>
         <stp xml:space="preserve">	JPY3M30Y=_x0003_BID_x0007_DTSIMI1ÿ_x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000_</stp>
         <tr r="Q38" s="7"/>
       </tp>
-      <tp>
-        <v>1.4851867670000001</v>
+      <tp t="s">
+        <v>#N/A Invalid source.</v>
         <stp/>
         <stp xml:space="preserve">	JPY3M25Y=_x0003_BID_x0007_DTSIMI1ÿ_x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000_</stp>
         <tr r="Q37" s="7"/>
       </tp>
-      <tp>
-        <v>1.313468232</v>
+      <tp t="s">
+        <v>#N/A Invalid source.</v>
         <stp/>
         <stp xml:space="preserve">	JPY3M20Y=_x0003_BID_x0007_DTSIMI1ÿ_x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000_</stp>
         <tr r="Q36" s="7"/>
       </tp>
-      <tp>
-        <v>0.99441074200000001</v>
+      <tp t="s">
+        <v>#N/A Invalid source.</v>
         <stp/>
         <stp xml:space="preserve">	JPY3M15Y=_x0003_BID_x0007_DTSIMI1ÿ_x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000_</stp>
         <tr r="Q35" s="7"/>
       </tp>
-      <tp>
-        <v>0.56303451500000001</v>
+      <tp t="s">
+        <v>#N/A Invalid source.</v>
         <stp/>
         <stp xml:space="preserve">	JPY3M10Y=_x0003_BID_x0007_DTSIMI1ÿ_x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000_</stp>
         <tr r="Q33" s="7"/>
       </tp>
-      <tp>
-        <v>0.74009947700000001</v>
+      <tp t="s">
+        <v>#N/A Invalid source.</v>
         <stp/>
         <stp xml:space="preserve">	JPY3M12Y=_x0003_BID_x0007_DTSIMI1ÿ_x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000_</stp>
         <tr r="Q34" s="7"/>
       </tp>
-      <tp>
-        <v>0.23113118199999999</v>
+      <tp t="s">
+        <v>#N/A Invalid source.</v>
         <stp/>
         <stp xml:space="preserve">	JPY6MSND=_x0003_ASK_x0007_DTSIMI1ÿ_x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000_</stp>
         <tr r="Y7" s="7"/>
       </tp>
-      <tp>
-        <v>0.23094794699999999</v>
+      <tp t="s">
+        <v>#N/A Invalid source.</v>
         <stp/>
         <stp xml:space="preserve">	JPY6MSWD=_x0003_ASK_x0007_DTSIMI1ÿ_x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000_</stp>
         <tr r="Y8" s="7"/>
       </tp>
-      <tp>
-        <v>0.231152212</v>
+      <tp t="s">
+        <v>#N/A Invalid source.</v>
         <stp/>
         <stp xml:space="preserve">	JPY6MTND=_x0003_ASK_x0007_DTSIMI1ÿ_x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000_</stp>
         <tr r="Y6" s="7"/>
       </tp>
-      <tp>
-        <v>0.231174873</v>
+      <tp t="s">
+        <v>#N/A Invalid source.</v>
         <stp/>
         <stp xml:space="preserve">	JPY6MOND=_x0003_ASK_x0007_DTSIMI1ÿ_x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000_</stp>
         <tr r="Y5" s="7"/>
       </tp>
-      <tp>
-        <v>0.2064</v>
+      <tp t="s">
+        <v>#N/A Invalid source.</v>
         <stp/>
         <stp xml:space="preserve">	JPY6M3MD=_x0003_ASK_x0007_DTSIMI1ÿ_x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000_</stp>
         <tr r="Y13" s="7"/>
       </tp>
-      <tp>
-        <v>0.229425409</v>
+      <tp t="s">
+        <v>#N/A Invalid source.</v>
         <stp/>
         <stp xml:space="preserve">	JPY6M3WD=_x0003_ASK_x0007_DTSIMI1ÿ_x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000_</stp>
         <tr r="Y10" s="7"/>
       </tp>
-      <tp>
-        <v>0.21729999999999999</v>
+      <tp t="s">
+        <v>#N/A Invalid source.</v>
         <stp/>
         <stp xml:space="preserve">	JPY6M2MD=_x0003_ASK_x0007_DTSIMI1ÿ_x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000_</stp>
         <tr r="Y12" s="7"/>
       </tp>
-      <tp>
-        <v>0.230378317</v>
+      <tp t="s">
+        <v>#N/A Invalid source.</v>
         <stp/>
         <stp xml:space="preserve">	JPY6M2WD=_x0003_ASK_x0007_DTSIMI1ÿ_x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000_</stp>
         <tr r="Y9" s="7"/>
       </tp>
-      <tp>
-        <v>0.22689999999999999</v>
+      <tp t="s">
+        <v>#N/A Invalid source.</v>
         <stp/>
         <stp xml:space="preserve">	JPY6M1MD=_x0003_ASK_x0007_DTSIMI1ÿ_x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000_</stp>
         <tr r="Y11" s="7"/>
       </tp>
-      <tp>
-        <v>0.1865</v>
+      <tp t="s">
+        <v>#N/A Invalid source.</v>
         <stp/>
         <stp xml:space="preserve">	JPY6M6MD=_x0003_ASK_x0007_DTSIMI1ÿ_x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000_</stp>
         <tr r="Y16" s="7"/>
       </tp>
-      <tp>
-        <v>0.19339999999999999</v>
+      <tp t="s">
+        <v>#N/A Invalid source.</v>
         <stp/>
         <stp xml:space="preserve">	JPY6M5MD=_x0003_ASK_x0007_DTSIMI1ÿ_x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000_</stp>
         <tr r="Y15" s="7"/>
       </tp>
-      <tp>
-        <v>0.19889999999999999</v>
+      <tp t="s">
+        <v>#N/A Invalid source.</v>
         <stp/>
         <stp xml:space="preserve">	JPY6M4MD=_x0003_ASK_x0007_DTSIMI1ÿ_x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000_</stp>
         <tr r="Y14" s="7"/>
       </tp>
-      <tp>
-        <v>1.73</v>
+      <tp t="s">
+        <v>#N/A Invalid source.</v>
         <stp/>
         <stp xml:space="preserve">	JPY6M30Y=_x0003_BID_x0007_DTSIMI1ÿ_x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000_</stp>
         <tr r="X38" s="7"/>
       </tp>
-      <tp>
-        <v>1.6274999999999999</v>
+      <tp t="s">
+        <v>#N/A Invalid source.</v>
         <stp/>
         <stp xml:space="preserve">	JPY6M25Y=_x0003_BID_x0007_DTSIMI1ÿ_x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000_</stp>
         <tr r="X37" s="7"/>
       </tp>
-      <tp>
-        <v>1.4550000000000001</v>
+      <tp t="s">
+        <v>#N/A Invalid source.</v>
         <stp/>
         <stp xml:space="preserve">	JPY6M20Y=_x0003_BID_x0007_DTSIMI1ÿ_x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000_</stp>
         <tr r="X36" s="7"/>
       </tp>
-      <tp>
-        <v>1.1325000000000001</v>
+      <tp t="s">
+        <v>#N/A Invalid source.</v>
         <stp/>
         <stp xml:space="preserve">	JPY6M15Y=_x0003_BID_x0007_DTSIMI1ÿ_x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000_</stp>
         <tr r="X35" s="7"/>
       </tp>
-      <tp>
-        <v>0.68</v>
+      <tp t="s">
+        <v>#N/A Invalid source.</v>
         <stp/>
         <stp xml:space="preserve">	JPY6M10Y=_x0003_BID_x0007_DTSIMI1ÿ_x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000_</stp>
         <tr r="X33" s="7"/>
       </tp>
-      <tp>
-        <v>0.86750000000000005</v>
+      <tp t="s">
+        <v>#N/A Invalid source.</v>
         <stp/>
         <stp xml:space="preserve">	JPY6M12Y=_x0003_BID_x0007_DTSIMI1ÿ_x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000_</stp>
         <tr r="X34" s="7"/>
       </tp>
-      <tp>
-        <v>0.138393131</v>
+      <tp t="s">
+        <v>#N/A Invalid source.</v>
         <stp/>
         <stp xml:space="preserve">	JPY3MSND=_x0003_ASK_x0007_DTSIMI1ÿ_x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000_</stp>
         <tr r="R7" s="7"/>
       </tp>
-      <tp>
-        <v>0.138377009</v>
+      <tp t="s">
+        <v>#N/A Invalid source.</v>
         <stp/>
         <stp xml:space="preserve">	JPY3MSWD=_x0003_ASK_x0007_DTSIMI1ÿ_x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000_</stp>
         <tr r="R8" s="7"/>
       </tp>
-      <tp>
-        <v>0.13840192900000001</v>
+      <tp t="s">
+        <v>#N/A Invalid source.</v>
         <stp/>
         <stp xml:space="preserve">	JPY3MTND=_x0003_ASK_x0007_DTSIMI1ÿ_x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000_</stp>
         <tr r="R6" s="7"/>
       </tp>
-      <tp>
-        <v>0.13840522499999999</v>
+      <tp t="s">
+        <v>#N/A Invalid source.</v>
         <stp/>
         <stp xml:space="preserve">	JPY3MOND=_x0003_ASK_x0007_DTSIMI1ÿ_x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000_</stp>
         <tr r="R5" s="7"/>
       </tp>
-      <tp>
-        <v>0.13250000000000001</v>
+      <tp t="s">
+        <v>#N/A Invalid source.</v>
         <stp/>
         <stp xml:space="preserve">	JPY3M3MD=_x0003_ASK_x0007_DTSIMI1ÿ_x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000_</stp>
         <tr r="R13" s="7"/>
       </tp>
-      <tp>
-        <v>0.13823602900000001</v>
+      <tp t="s">
+        <v>#N/A Invalid source.</v>
         <stp/>
         <stp xml:space="preserve">	JPY3M3WD=_x0003_ASK_x0007_DTSIMI1ÿ_x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000_</stp>
         <tr r="R10" s="7"/>
       </tp>
-      <tp>
-        <v>0.1361</v>
+      <tp t="s">
+        <v>#N/A Invalid source.</v>
         <stp/>
         <stp xml:space="preserve">	JPY3M2MD=_x0003_ASK_x0007_DTSIMI1ÿ_x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000_</stp>
         <tr r="R12" s="7"/>
       </tp>
-      <tp>
-        <v>0.13832460899999999</v>
+      <tp t="s">
+        <v>#N/A Invalid source.</v>
         <stp/>
         <stp xml:space="preserve">	JPY3M2WD=_x0003_ASK_x0007_DTSIMI1ÿ_x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000_</stp>
         <tr r="R9" s="7"/>
       </tp>
-      <tp>
-        <v>0.13800000000000001</v>
+      <tp t="s">
+        <v>#N/A Invalid source.</v>
         <stp/>
         <stp xml:space="preserve">	JPY3M1MD=_x0003_ASK_x0007_DTSIMI1ÿ_x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000_</stp>
         <tr r="R11" s="7"/>
       </tp>
-      <tp>
-        <v>5.6712328999999999E-2</v>
+      <tp t="s">
+        <v>#N/A Invalid source.</v>
         <stp/>
         <stp>_x000B_JPYON1Y6MD=_x0003_ASK_x0007_DTSIMI1ÿ_x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000_</stp>
         <tr r="K24" s="7"/>
       </tp>
-      <tp>
-        <v>5.6712328999999999E-2</v>
+      <tp t="s">
+        <v>#N/A Invalid source.</v>
         <stp/>
         <stp>_x000B_JPYON1Y6MD=_x0003_BID_x0007_DTSIMI1ÿ_x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000_</stp>
         <tr r="J24" s="7"/>
       </tp>
-      <tp>
-        <v>0.16500000000000001</v>
+      <tp t="s">
+        <v>#N/A Invalid source.</v>
         <stp/>
         <stp>_x000B_JPY6M5x11F=_x0003_BID_x0007_DTSIMI1ÿ_x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000_</stp>
         <tr r="X21" s="7"/>
       </tp>
-      <tp>
-        <v>0.16500000000000001</v>
+      <tp t="s">
+        <v>#N/A Invalid source.</v>
         <stp/>
         <stp>_x000B_JPY6M6x12F=_x0003_ASK_x0007_DTSIMI1ÿ_x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000_</stp>
         <tr r="Y22" s="7"/>
       </tp>
-      <tp>
-        <v>0.17</v>
+      <tp t="s">
+        <v>#N/A Invalid source.</v>
         <stp/>
         <stp>_x000B_JPY6M4x10F=_x0003_BID_x0007_DTSIMI1ÿ_x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000_</stp>
         <tr r="X20" s="7"/>
       </tp>
-      <tp>
-        <v>0.17</v>
+      <tp t="s">
+        <v>#N/A Invalid source.</v>
         <stp/>
         <stp>_x000B_JPY6M4x10F=_x0003_ASK_x0007_DTSIMI1ÿ_x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000_</stp>
         <tr r="Y20" s="7"/>
       </tp>
-      <tp>
-        <v>0.16500000000000001</v>
+      <tp t="s">
+        <v>#N/A Invalid source.</v>
         <stp/>
         <stp>_x000B_JPY6M6x12F=_x0003_BID_x0007_DTSIMI1ÿ_x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000_</stp>
         <tr r="X22" s="7"/>
       </tp>
-      <tp>
-        <v>0.16500000000000001</v>
+      <tp t="s">
+        <v>#N/A Invalid source.</v>
         <stp/>
         <stp>_x000B_JPY6M5x11F=_x0003_ASK_x0007_DTSIMI1ÿ_x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000_</stp>
         <tr r="Y21" s="7"/>
       </tp>
-      <tp>
-        <v>0.115</v>
+      <tp t="s">
+        <v>#N/A Invalid source.</v>
         <stp/>
         <stp>_x000B_JPY3M9x12F=_x0003_ASK_x0007_DTSIMI1ÿ_x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000_</stp>
         <tr r="R22" s="7"/>
       </tp>
-      <tp>
-        <v>0.115</v>
+      <tp t="s">
+        <v>#N/A Invalid source.</v>
         <stp/>
         <stp>_x000B_JPY3M9x12F=_x0003_BID_x0007_DTSIMI1ÿ_x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000_</stp>
         <tr r="Q22" s="7"/>
@@ -2625,7 +2637,7 @@
       <sheetData sheetId="0">
         <row r="7">
           <cell r="D7">
-            <v>3</v>
+            <v>2</v>
           </cell>
         </row>
       </sheetData>
@@ -3219,7 +3231,7 @@
       </c>
       <c r="D6" s="133">
         <f>[1]!TriggerCounter</f>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E6" s="131"/>
       <c r="F6" s="2"/>
@@ -6303,13 +6315,13 @@
         <f>H5</f>
         <v>6.42807346373786E-2</v>
       </c>
-      <c r="J5" s="18">
+      <c r="J5" s="18" t="e">
         <f>ABS(_xll.RtGet(SourceAlias,$G5,BID)-H5)</f>
-        <v>6.3737859434809252E-10</v>
-      </c>
-      <c r="K5" s="18">
+        <v>#VALUE!</v>
+      </c>
+      <c r="K5" s="18" t="e">
         <f>ABS(_xll.RtGet(SourceAlias,$G5,ASK)-I5)</f>
-        <v>6.3737859434809252E-10</v>
+        <v>#VALUE!</v>
       </c>
       <c r="L5" s="68" t="s">
         <v>120</v>
@@ -6329,13 +6341,13 @@
         <f>O5</f>
         <v>0.13840522543938463</v>
       </c>
-      <c r="Q5" s="18">
+      <c r="Q5" s="18" t="e">
         <f>ABS(_xll.RtGet(SourceAlias,$N5,BID)-O5)</f>
-        <v>4.3938463978321352E-10</v>
-      </c>
-      <c r="R5" s="18">
+        <v>#VALUE!</v>
+      </c>
+      <c r="R5" s="18" t="e">
         <f>ABS(_xll.RtGet(SourceAlias,$N5,ASK)-P5)</f>
-        <v>4.3938463978321352E-10</v>
+        <v>#VALUE!</v>
       </c>
       <c r="S5" s="68" t="s">
         <v>120</v>
@@ -6355,13 +6367,13 @@
         <f>V5</f>
         <v>0.13648556421825372</v>
       </c>
-      <c r="X5" s="18">
+      <c r="X5" s="18" t="e">
         <f>ABS(_xll.RtGet(SourceAlias,$U5,BID)-V5)</f>
-        <v>9.4689308781746279E-2</v>
-      </c>
-      <c r="Y5" s="18">
+        <v>#VALUE!</v>
+      </c>
+      <c r="Y5" s="18" t="e">
         <f>ABS(_xll.RtGet(SourceAlias,$U5,ASK)-W5)</f>
-        <v>9.4689308781746279E-2</v>
+        <v>#VALUE!</v>
       </c>
       <c r="Z5" s="2"/>
       <c r="AA5" s="2"/>
@@ -6425,13 +6437,13 @@
         <f t="shared" ref="I6:I38" si="3">H6</f>
         <v>6.4284050872887022E-2</v>
       </c>
-      <c r="J6" s="20">
+      <c r="J6" s="20" t="e">
         <f>ABS(_xll.RtGet(SourceAlias,$G6,BID)-H6)</f>
-        <v>1.2711297292522516E-10</v>
-      </c>
-      <c r="K6" s="20">
+        <v>#VALUE!</v>
+      </c>
+      <c r="K6" s="20" t="e">
         <f>ABS(_xll.RtGet(SourceAlias,$G6,ASK)-I6)</f>
-        <v>1.2711297292522516E-10</v>
+        <v>#VALUE!</v>
       </c>
       <c r="L6" s="68" t="s">
         <v>120</v>
@@ -6451,13 +6463,13 @@
         <f t="shared" ref="P6:P38" si="4">O6</f>
         <v>0.13840192914472738</v>
       </c>
-      <c r="Q6" s="20">
+      <c r="Q6" s="20" t="e">
         <f>ABS(_xll.RtGet(SourceAlias,$N6,BID)-O6)</f>
-        <v>1.4472736897808147E-10</v>
-      </c>
-      <c r="R6" s="20">
+        <v>#VALUE!</v>
+      </c>
+      <c r="R6" s="20" t="e">
         <f>ABS(_xll.RtGet(SourceAlias,$N6,ASK)-P6)</f>
-        <v>1.4472736897808147E-10</v>
+        <v>#VALUE!</v>
       </c>
       <c r="S6" s="68" t="s">
         <v>120</v>
@@ -6477,13 +6489,13 @@
         <f t="shared" ref="W6:W38" si="5">V6</f>
         <v>0.13651789399230593</v>
       </c>
-      <c r="X6" s="20">
+      <c r="X6" s="20" t="e">
         <f>ABS(_xll.RtGet(SourceAlias,$U6,BID)-V6)</f>
-        <v>9.4634318007694063E-2</v>
-      </c>
-      <c r="Y6" s="20">
+        <v>#VALUE!</v>
+      </c>
+      <c r="Y6" s="20" t="e">
         <f>ABS(_xll.RtGet(SourceAlias,$U6,ASK)-W6)</f>
-        <v>9.4634318007694063E-2</v>
+        <v>#VALUE!</v>
       </c>
       <c r="Z6" s="2"/>
       <c r="AA6" s="2"/>
@@ -6547,13 +6559,13 @@
         <f t="shared" si="3"/>
         <v>6.4290683352008493E-2</v>
       </c>
-      <c r="J7" s="22">
+      <c r="J7" s="22" t="e">
         <f>ABS(_xll.RtGet(SourceAlias,$G7,BID)-H7)</f>
-        <v>3.520084917996158E-10</v>
-      </c>
-      <c r="K7" s="22">
+        <v>#VALUE!</v>
+      </c>
+      <c r="K7" s="22" t="e">
         <f>ABS(_xll.RtGet(SourceAlias,$G7,ASK)-I7)</f>
-        <v>3.520084917996158E-10</v>
+        <v>#VALUE!</v>
       </c>
       <c r="L7" s="68" t="s">
         <v>120</v>
@@ -6573,13 +6585,13 @@
         <f t="shared" si="4"/>
         <v>0.13839313119490271</v>
       </c>
-      <c r="Q7" s="22">
+      <c r="Q7" s="22" t="e">
         <f>ABS(_xll.RtGet(SourceAlias,$N7,BID)-O7)</f>
-        <v>1.9490270508626395E-10</v>
-      </c>
-      <c r="R7" s="22">
+        <v>#VALUE!</v>
+      </c>
+      <c r="R7" s="22" t="e">
         <f>ABS(_xll.RtGet(SourceAlias,$N7,ASK)-P7)</f>
-        <v>1.9490270508626395E-10</v>
+        <v>#VALUE!</v>
       </c>
       <c r="S7" s="68" t="s">
         <v>120</v>
@@ -6599,13 +6611,13 @@
         <f t="shared" si="5"/>
         <v>0.13654796993112228</v>
       </c>
-      <c r="X7" s="22">
+      <c r="X7" s="22" t="e">
         <f>ABS(_xll.RtGet(SourceAlias,$U7,BID)-V7)</f>
-        <v>9.4583212068877709E-2</v>
-      </c>
-      <c r="Y7" s="22">
+        <v>#VALUE!</v>
+      </c>
+      <c r="Y7" s="22" t="e">
         <f>ABS(_xll.RtGet(SourceAlias,$U7,ASK)-W7)</f>
-        <v>9.4583212068877709E-2</v>
+        <v>#VALUE!</v>
       </c>
       <c r="Z7" s="2"/>
       <c r="AA7" s="2"/>
@@ -6669,13 +6681,13 @@
         <f t="shared" si="3"/>
         <v>6.345611596067105E-2</v>
       </c>
-      <c r="J8" s="20">
+      <c r="J8" s="20" t="e">
         <f>ABS(_xll.RtGet(SourceAlias,$G8,BID)-H8)</f>
-        <v>3.932895675795578E-11</v>
-      </c>
-      <c r="K8" s="20">
+        <v>#VALUE!</v>
+      </c>
+      <c r="K8" s="20" t="e">
         <f>ABS(_xll.RtGet(SourceAlias,$G8,ASK)-I8)</f>
-        <v>3.932895675795578E-11</v>
+        <v>#VALUE!</v>
       </c>
       <c r="L8" s="68" t="s">
         <v>120</v>
@@ -6695,13 +6707,13 @@
         <f t="shared" si="4"/>
         <v>0.13837700945096287</v>
       </c>
-      <c r="Q8" s="20">
+      <c r="Q8" s="20" t="e">
         <f>ABS(_xll.RtGet(SourceAlias,$N8,BID)-O8)</f>
-        <v>4.5096287815127312E-10</v>
-      </c>
-      <c r="R8" s="20">
+        <v>#VALUE!</v>
+      </c>
+      <c r="R8" s="20" t="e">
         <f>ABS(_xll.RtGet(SourceAlias,$N8,ASK)-P8)</f>
-        <v>4.5096287815127312E-10</v>
+        <v>#VALUE!</v>
       </c>
       <c r="S8" s="68" t="s">
         <v>120</v>
@@ -6721,13 +6733,13 @@
         <f t="shared" si="5"/>
         <v>0.13680730979727582</v>
       </c>
-      <c r="X8" s="20">
+      <c r="X8" s="20" t="e">
         <f>ABS(_xll.RtGet(SourceAlias,$U8,BID)-V8)</f>
-        <v>9.414063720272417E-2</v>
-      </c>
-      <c r="Y8" s="20">
+        <v>#VALUE!</v>
+      </c>
+      <c r="Y8" s="20" t="e">
         <f>ABS(_xll.RtGet(SourceAlias,$U8,ASK)-W8)</f>
-        <v>9.414063720272417E-2</v>
+        <v>#VALUE!</v>
       </c>
       <c r="Z8" s="2"/>
       <c r="AA8" s="2"/>
@@ -6791,13 +6803,13 @@
         <f t="shared" si="3"/>
         <v>6.3559540343443327E-2</v>
       </c>
-      <c r="J9" s="20">
+      <c r="J9" s="20" t="e">
         <f>ABS(_xll.RtGet(SourceAlias,$G9,BID)-H9)</f>
-        <v>3.4344332933144983E-10</v>
-      </c>
-      <c r="K9" s="20">
+        <v>#VALUE!</v>
+      </c>
+      <c r="K9" s="20" t="e">
         <f>ABS(_xll.RtGet(SourceAlias,$G9,ASK)-I9)</f>
-        <v>3.4344332933144983E-10</v>
+        <v>#VALUE!</v>
       </c>
       <c r="L9" s="68" t="s">
         <v>120</v>
@@ -6817,13 +6829,13 @@
         <f t="shared" si="4"/>
         <v>0.13832460881970018</v>
       </c>
-      <c r="Q9" s="20">
+      <c r="Q9" s="20" t="e">
         <f>ABS(_xll.RtGet(SourceAlias,$N9,BID)-O9)</f>
-        <v>1.8029980286549119E-10</v>
-      </c>
-      <c r="R9" s="20">
+        <v>#VALUE!</v>
+      </c>
+      <c r="R9" s="20" t="e">
         <f>ABS(_xll.RtGet(SourceAlias,$N9,ASK)-P9)</f>
-        <v>1.8029980286549119E-10</v>
+        <v>#VALUE!</v>
       </c>
       <c r="S9" s="68" t="s">
         <v>120</v>
@@ -6843,13 +6855,13 @@
         <f t="shared" si="5"/>
         <v>0.13759862044514037</v>
       </c>
-      <c r="X9" s="20">
+      <c r="X9" s="20" t="e">
         <f>ABS(_xll.RtGet(SourceAlias,$U9,BID)-V9)</f>
-        <v>9.2779696554859625E-2</v>
-      </c>
-      <c r="Y9" s="20">
+        <v>#VALUE!</v>
+      </c>
+      <c r="Y9" s="20" t="e">
         <f>ABS(_xll.RtGet(SourceAlias,$U9,ASK)-W9)</f>
-        <v>9.2779696554859625E-2</v>
+        <v>#VALUE!</v>
       </c>
       <c r="Z9" s="2"/>
       <c r="AA9" s="2"/>
@@ -6913,13 +6925,13 @@
         <f t="shared" si="3"/>
         <v>6.371639241249076E-2</v>
       </c>
-      <c r="J10" s="20">
+      <c r="J10" s="20" t="e">
         <f>ABS(_xll.RtGet(SourceAlias,$G10,BID)-H10)</f>
-        <v>4.1249076376814742E-10</v>
-      </c>
-      <c r="K10" s="20">
+        <v>#VALUE!</v>
+      </c>
+      <c r="K10" s="20" t="e">
         <f>ABS(_xll.RtGet(SourceAlias,$G10,ASK)-I10)</f>
-        <v>4.1249076376814742E-10</v>
+        <v>#VALUE!</v>
       </c>
       <c r="L10" s="68" t="s">
         <v>120</v>
@@ -6939,13 +6951,13 @@
         <f t="shared" si="4"/>
         <v>0.13823602949182753</v>
       </c>
-      <c r="Q10" s="20">
+      <c r="Q10" s="20" t="e">
         <f>ABS(_xll.RtGet(SourceAlias,$N10,BID)-O10)</f>
-        <v>4.9182752315246603E-10</v>
-      </c>
-      <c r="R10" s="20">
+        <v>#VALUE!</v>
+      </c>
+      <c r="R10" s="20" t="e">
         <f>ABS(_xll.RtGet(SourceAlias,$N10,ASK)-P10)</f>
-        <v>4.9182752315246603E-10</v>
+        <v>#VALUE!</v>
       </c>
       <c r="S10" s="68" t="s">
         <v>120</v>
@@ -6965,13 +6977,13 @@
         <f t="shared" si="5"/>
         <v>0.1389163154409242</v>
       </c>
-      <c r="X10" s="20">
+      <c r="X10" s="20" t="e">
         <f>ABS(_xll.RtGet(SourceAlias,$U10,BID)-V10)</f>
-        <v>9.0509093559075798E-2</v>
-      </c>
-      <c r="Y10" s="20">
+        <v>#VALUE!</v>
+      </c>
+      <c r="Y10" s="20" t="e">
         <f>ABS(_xll.RtGet(SourceAlias,$U10,ASK)-W10)</f>
-        <v>9.0509093559075798E-2</v>
+        <v>#VALUE!</v>
       </c>
       <c r="Z10" s="2"/>
       <c r="AA10" s="2"/>
@@ -7035,13 +7047,13 @@
         <f t="shared" si="3"/>
         <v>6.4109588627125888E-2</v>
       </c>
-      <c r="J11" s="20">
+      <c r="J11" s="20" t="e">
         <f>ABS(_xll.RtGet(SourceAlias,$G11,BID)-H11)</f>
-        <v>3.7287410659114784E-10</v>
-      </c>
-      <c r="K11" s="20">
+        <v>#VALUE!</v>
+      </c>
+      <c r="K11" s="20" t="e">
         <f>ABS(_xll.RtGet(SourceAlias,$G11,ASK)-I11)</f>
-        <v>3.7287410659114784E-10</v>
+        <v>#VALUE!</v>
       </c>
       <c r="L11" s="68" t="s">
         <v>120</v>
@@ -7061,13 +7073,13 @@
         <f t="shared" si="4"/>
         <v>0.13799999999991094</v>
       </c>
-      <c r="Q11" s="20">
+      <c r="Q11" s="20" t="e">
         <f>ABS(_xll.RtGet(SourceAlias,$N11,BID)-O11)</f>
-        <v>8.9067642150553183E-14</v>
-      </c>
-      <c r="R11" s="20">
+        <v>#VALUE!</v>
+      </c>
+      <c r="R11" s="20" t="e">
         <f>ABS(_xll.RtGet(SourceAlias,$N11,ASK)-P11)</f>
-        <v>8.9067642150553183E-14</v>
+        <v>#VALUE!</v>
       </c>
       <c r="S11" s="68" t="s">
         <v>120</v>
@@ -7087,13 +7099,13 @@
         <f t="shared" si="5"/>
         <v>0.14239999999989614</v>
       </c>
-      <c r="X11" s="20">
+      <c r="X11" s="20" t="e">
         <f>ABS(_xll.RtGet(SourceAlias,$U11,BID)-V11)</f>
-        <v>8.4500000000103853E-2</v>
-      </c>
-      <c r="Y11" s="20">
+        <v>#VALUE!</v>
+      </c>
+      <c r="Y11" s="20" t="e">
         <f>ABS(_xll.RtGet(SourceAlias,$U11,ASK)-W11)</f>
-        <v>8.4500000000103853E-2</v>
+        <v>#VALUE!</v>
       </c>
       <c r="Z11" s="2"/>
       <c r="AA11" s="2"/>
@@ -7157,13 +7169,13 @@
         <f t="shared" si="3"/>
         <v>6.4109588628372238E-2</v>
       </c>
-      <c r="J12" s="20">
+      <c r="J12" s="20" t="e">
         <f>ABS(_xll.RtGet(SourceAlias,$G12,BID)-H12)</f>
-        <v>3.7162775634591583E-10</v>
-      </c>
-      <c r="K12" s="20">
+        <v>#VALUE!</v>
+      </c>
+      <c r="K12" s="20" t="e">
         <f>ABS(_xll.RtGet(SourceAlias,$G12,ASK)-I12)</f>
-        <v>3.7162775634591583E-10</v>
+        <v>#VALUE!</v>
       </c>
       <c r="L12" s="68" t="s">
         <v>120</v>
@@ -7183,13 +7195,13 @@
         <f t="shared" si="4"/>
         <v>0.13609999999990788</v>
       </c>
-      <c r="Q12" s="20">
+      <c r="Q12" s="20" t="e">
         <f>ABS(_xll.RtGet(SourceAlias,$N12,BID)-O12)</f>
-        <v>9.2120755468272364E-14</v>
-      </c>
-      <c r="R12" s="20">
+        <v>#VALUE!</v>
+      </c>
+      <c r="R12" s="20" t="e">
         <f>ABS(_xll.RtGet(SourceAlias,$N12,ASK)-P12)</f>
-        <v>9.2120755468272364E-14</v>
+        <v>#VALUE!</v>
       </c>
       <c r="S12" s="68" t="s">
         <v>120</v>
@@ -7209,13 +7221,13 @@
         <f t="shared" si="5"/>
         <v>0.15249999999999986</v>
       </c>
-      <c r="X12" s="20">
+      <c r="X12" s="20" t="e">
         <f>ABS(_xll.RtGet(SourceAlias,$U12,BID)-V12)</f>
-        <v>6.4800000000000135E-2</v>
-      </c>
-      <c r="Y12" s="20">
+        <v>#VALUE!</v>
+      </c>
+      <c r="Y12" s="20" t="e">
         <f>ABS(_xll.RtGet(SourceAlias,$U12,ASK)-W12)</f>
-        <v>6.4800000000000135E-2</v>
+        <v>#VALUE!</v>
       </c>
       <c r="Z12" s="2"/>
       <c r="AA12" s="2"/>
@@ -7279,13 +7291,13 @@
         <f t="shared" si="3"/>
         <v>6.1643835914130307E-2</v>
       </c>
-      <c r="J13" s="20">
+      <c r="J13" s="20" t="e">
         <f>ABS(_xll.RtGet(SourceAlias,$G13,BID)-H13)</f>
-        <v>8.5869693300377747E-11</v>
-      </c>
-      <c r="K13" s="20">
+        <v>#VALUE!</v>
+      </c>
+      <c r="K13" s="20" t="e">
         <f>ABS(_xll.RtGet(SourceAlias,$G13,ASK)-I13)</f>
-        <v>8.5869693300377747E-11</v>
+        <v>#VALUE!</v>
       </c>
       <c r="L13" s="68" t="s">
         <v>120</v>
@@ -7305,13 +7317,13 @@
         <f t="shared" si="4"/>
         <v>0.13250000000238857</v>
       </c>
-      <c r="Q13" s="20">
+      <c r="Q13" s="20" t="e">
         <f>ABS(_xll.RtGet(SourceAlias,$N13,BID)-O13)</f>
-        <v>2.3885615707541774E-12</v>
-      </c>
-      <c r="R13" s="20">
+        <v>#VALUE!</v>
+      </c>
+      <c r="R13" s="20" t="e">
         <f>ABS(_xll.RtGet(SourceAlias,$N13,ASK)-P13)</f>
-        <v>2.3885615707541774E-12</v>
+        <v>#VALUE!</v>
       </c>
       <c r="S13" s="68" t="s">
         <v>120</v>
@@ -7331,13 +7343,13 @@
         <f t="shared" si="5"/>
         <v>0.15850000000005657</v>
       </c>
-      <c r="X13" s="20">
+      <c r="X13" s="20" t="e">
         <f>ABS(_xll.RtGet(SourceAlias,$U13,BID)-V13)</f>
-        <v>4.7899999999943432E-2</v>
-      </c>
-      <c r="Y13" s="20">
+        <v>#VALUE!</v>
+      </c>
+      <c r="Y13" s="20" t="e">
         <f>ABS(_xll.RtGet(SourceAlias,$U13,ASK)-W13)</f>
-        <v>4.7899999999943432E-2</v>
+        <v>#VALUE!</v>
       </c>
       <c r="Z13" s="2"/>
       <c r="AA13" s="2"/>
@@ -7401,13 +7413,13 @@
         <f t="shared" si="3"/>
         <v>6.1643835730187682E-2</v>
       </c>
-      <c r="J14" s="20">
+      <c r="J14" s="20" t="e">
         <f>ABS(_xll.RtGet(SourceAlias,$G14,BID)-H14)</f>
-        <v>2.6981231832090558E-10</v>
-      </c>
-      <c r="K14" s="20">
+        <v>#VALUE!</v>
+      </c>
+      <c r="K14" s="20" t="e">
         <f>ABS(_xll.RtGet(SourceAlias,$G14,ASK)-I14)</f>
-        <v>2.6981231832090558E-10</v>
+        <v>#VALUE!</v>
       </c>
       <c r="L14" s="68" t="s">
         <v>120</v>
@@ -7427,13 +7439,13 @@
         <f t="shared" si="4"/>
         <v>0.1300000000000697</v>
       </c>
-      <c r="Q14" s="20">
+      <c r="Q14" s="20" t="e">
         <f>ABS(_xll.RtGet(SourceAlias,$N14,BID)-O14)</f>
-        <v>6.9694250370844202E-14</v>
-      </c>
-      <c r="R14" s="20">
+        <v>#VALUE!</v>
+      </c>
+      <c r="R14" s="20" t="e">
         <f>ABS(_xll.RtGet(SourceAlias,$N14,ASK)-P14)</f>
-        <v>6.9694250370844202E-14</v>
+        <v>#VALUE!</v>
       </c>
       <c r="S14" s="68" t="s">
         <v>120</v>
@@ -7453,13 +7465,13 @@
         <f t="shared" si="5"/>
         <v>0.16549999999996901</v>
       </c>
-      <c r="X14" s="20">
+      <c r="X14" s="20" t="e">
         <f>ABS(_xll.RtGet(SourceAlias,$U14,BID)-V14)</f>
-        <v>3.3400000000030988E-2</v>
-      </c>
-      <c r="Y14" s="20">
+        <v>#VALUE!</v>
+      </c>
+      <c r="Y14" s="20" t="e">
         <f>ABS(_xll.RtGet(SourceAlias,$U14,ASK)-W14)</f>
-        <v>3.3400000000030988E-2</v>
+        <v>#VALUE!</v>
       </c>
       <c r="Z14" s="2"/>
       <c r="AA14" s="2"/>
@@ -7523,13 +7535,13 @@
         <f t="shared" si="3"/>
         <v>6.164383573323437E-2</v>
       </c>
-      <c r="J15" s="20">
+      <c r="J15" s="20" t="e">
         <f>ABS(_xll.RtGet(SourceAlias,$G15,BID)-H15)</f>
-        <v>2.6676563041894141E-10</v>
-      </c>
-      <c r="K15" s="20">
+        <v>#VALUE!</v>
+      </c>
+      <c r="K15" s="20" t="e">
         <f>ABS(_xll.RtGet(SourceAlias,$G15,ASK)-I15)</f>
-        <v>2.6676563041894141E-10</v>
+        <v>#VALUE!</v>
       </c>
       <c r="L15" s="68" t="s">
         <v>120</v>
@@ -7549,13 +7561,13 @@
         <f t="shared" si="4"/>
         <v>0.12999999999992934</v>
       </c>
-      <c r="Q15" s="20">
+      <c r="Q15" s="20" t="e">
         <f>ABS(_xll.RtGet(SourceAlias,$N15,BID)-O15)</f>
-        <v>7.0665695517391214E-14</v>
-      </c>
-      <c r="R15" s="20">
+        <v>#VALUE!</v>
+      </c>
+      <c r="R15" s="20" t="e">
         <f>ABS(_xll.RtGet(SourceAlias,$N15,ASK)-P15)</f>
-        <v>7.0665695517391214E-14</v>
+        <v>#VALUE!</v>
       </c>
       <c r="S15" s="68" t="s">
         <v>120</v>
@@ -7575,13 +7587,13 @@
         <f t="shared" si="5"/>
         <v>0.16989999999997121</v>
       </c>
-      <c r="X15" s="20">
+      <c r="X15" s="20" t="e">
         <f>ABS(_xll.RtGet(SourceAlias,$U15,BID)-V15)</f>
-        <v>2.3500000000028776E-2</v>
-      </c>
-      <c r="Y15" s="20">
+        <v>#VALUE!</v>
+      </c>
+      <c r="Y15" s="20" t="e">
         <f>ABS(_xll.RtGet(SourceAlias,$U15,ASK)-W15)</f>
-        <v>2.3500000000028776E-2</v>
+        <v>#VALUE!</v>
       </c>
       <c r="Z15" s="2"/>
       <c r="AA15" s="2"/>
@@ -7645,13 +7657,13 @@
         <f t="shared" si="3"/>
         <v>5.9178082285113821E-2</v>
       </c>
-      <c r="J16" s="20">
+      <c r="J16" s="20" t="e">
         <f>ABS(_xll.RtGet(SourceAlias,$G16,BID)-H16)</f>
-        <v>2.8511382144102981E-10</v>
-      </c>
-      <c r="K16" s="20">
+        <v>#VALUE!</v>
+      </c>
+      <c r="K16" s="20" t="e">
         <f>ABS(_xll.RtGet(SourceAlias,$G16,ASK)-I16)</f>
-        <v>2.8511382144102981E-10</v>
+        <v>#VALUE!</v>
       </c>
       <c r="L16" s="68" t="s">
         <v>120</v>
@@ -7671,13 +7683,13 @@
         <f t="shared" si="4"/>
         <v>0.13000000001058301</v>
       </c>
-      <c r="Q16" s="20">
+      <c r="Q16" s="20" t="e">
         <f>ABS(_xll.RtGet(SourceAlias,$N16,BID)-O16)</f>
-        <v>1.0583006693209995E-11</v>
-      </c>
-      <c r="R16" s="20">
+        <v>#VALUE!</v>
+      </c>
+      <c r="R16" s="20" t="e">
         <f>ABS(_xll.RtGet(SourceAlias,$N16,ASK)-P16)</f>
-        <v>1.0583006693209995E-11</v>
+        <v>#VALUE!</v>
       </c>
       <c r="S16" s="68" t="s">
         <v>120</v>
@@ -7697,13 +7709,13 @@
         <f t="shared" si="5"/>
         <v>0.17009999992740985</v>
       </c>
-      <c r="X16" s="20">
+      <c r="X16" s="20" t="e">
         <f>ABS(_xll.RtGet(SourceAlias,$U16,BID)-V16)</f>
-        <v>1.6400000072590154E-2</v>
-      </c>
-      <c r="Y16" s="20">
+        <v>#VALUE!</v>
+      </c>
+      <c r="Y16" s="20" t="e">
         <f>ABS(_xll.RtGet(SourceAlias,$U16,ASK)-W16)</f>
-        <v>1.6400000072590154E-2</v>
+        <v>#VALUE!</v>
       </c>
       <c r="Z16" s="2"/>
       <c r="AA16" s="2"/>
@@ -7773,13 +7785,13 @@
         <f t="shared" si="4"/>
         <v>0.12500000000003694</v>
       </c>
-      <c r="Q17" s="20">
+      <c r="Q17" s="20" t="e">
         <f>ABS(_xll.RtGet(SourceAlias,$N17,BID)-O17)</f>
-        <v>3.6942671144402084E-14</v>
-      </c>
-      <c r="R17" s="20">
+        <v>#VALUE!</v>
+      </c>
+      <c r="R17" s="20" t="e">
         <f>ABS(_xll.RtGet(SourceAlias,$N17,ASK)-P17)</f>
-        <v>3.6942671144402084E-14</v>
+        <v>#VALUE!</v>
       </c>
       <c r="S17" s="68" t="s">
         <v>120</v>
@@ -7799,13 +7811,13 @@
         <f t="shared" si="5"/>
         <v>0.17499999999997351</v>
       </c>
-      <c r="X17" s="20">
+      <c r="X17" s="20" t="e">
         <f>ABS(_xll.RtGet(SourceAlias,$U17,BID)-V17)</f>
-        <v>2.6478819137309983E-14</v>
-      </c>
-      <c r="Y17" s="20">
+        <v>#VALUE!</v>
+      </c>
+      <c r="Y17" s="20" t="e">
         <f>ABS(_xll.RtGet(SourceAlias,$U17,ASK)-W17)</f>
-        <v>2.6478819137309983E-14</v>
+        <v>#VALUE!</v>
       </c>
       <c r="Z17" s="2"/>
       <c r="AA17" s="2"/>
@@ -7877,13 +7889,13 @@
         <f t="shared" si="4"/>
         <v>0.12500000000006395</v>
       </c>
-      <c r="Q18" s="20">
+      <c r="Q18" s="20" t="e">
         <f>ABS(_xll.RtGet(SourceAlias,$N18,BID)-O18)</f>
-        <v>6.3948846218409017E-14</v>
-      </c>
-      <c r="R18" s="20">
+        <v>#VALUE!</v>
+      </c>
+      <c r="R18" s="20" t="e">
         <f>ABS(_xll.RtGet(SourceAlias,$N18,ASK)-P18)</f>
-        <v>6.3948846218409017E-14</v>
+        <v>#VALUE!</v>
       </c>
       <c r="S18" s="68" t="s">
         <v>120</v>
@@ -7903,13 +7915,13 @@
         <f t="shared" si="5"/>
         <v>0.1749999999999651</v>
       </c>
-      <c r="X18" s="20">
+      <c r="X18" s="20" t="e">
         <f>ABS(_xll.RtGet(SourceAlias,$U18,BID)-V18)</f>
-        <v>3.4888758548845544E-14</v>
-      </c>
-      <c r="Y18" s="20">
+        <v>#VALUE!</v>
+      </c>
+      <c r="Y18" s="20" t="e">
         <f>ABS(_xll.RtGet(SourceAlias,$U18,ASK)-W18)</f>
-        <v>3.4888758548845544E-14</v>
+        <v>#VALUE!</v>
       </c>
       <c r="Z18" s="2"/>
       <c r="AA18" s="2"/>
@@ -7973,13 +7985,13 @@
         <f t="shared" si="3"/>
         <v>5.9178082254617091E-2</v>
       </c>
-      <c r="J19" s="20">
+      <c r="J19" s="20" t="e">
         <f>ABS(_xll.RtGet(SourceAlias,$G19,BID)-H19)</f>
-        <v>2.5461709129981358E-10</v>
-      </c>
-      <c r="K19" s="20">
+        <v>#VALUE!</v>
+      </c>
+      <c r="K19" s="20" t="e">
         <f>ABS(_xll.RtGet(SourceAlias,$G19,ASK)-I19)</f>
-        <v>2.5461709129981358E-10</v>
+        <v>#VALUE!</v>
       </c>
       <c r="L19" s="68" t="s">
         <v>120</v>
@@ -7999,13 +8011,13 @@
         <f t="shared" si="4"/>
         <v>0.12500000004003198</v>
       </c>
-      <c r="Q19" s="20">
+      <c r="Q19" s="20" t="e">
         <f>ABS(_xll.RtGet(SourceAlias,$N19,BID)-O19)</f>
-        <v>4.0031977732724044E-11</v>
-      </c>
-      <c r="R19" s="20">
+        <v>#VALUE!</v>
+      </c>
+      <c r="R19" s="20" t="e">
         <f>ABS(_xll.RtGet(SourceAlias,$N19,ASK)-P19)</f>
-        <v>4.0031977732724044E-11</v>
+        <v>#VALUE!</v>
       </c>
       <c r="S19" s="68" t="s">
         <v>120</v>
@@ -8025,13 +8037,13 @@
         <f t="shared" si="5"/>
         <v>0.17000000000001569</v>
       </c>
-      <c r="X19" s="20">
+      <c r="X19" s="20" t="e">
         <f>ABS(_xll.RtGet(SourceAlias,$U19,BID)-V19)</f>
-        <v>1.5681900222830336E-14</v>
-      </c>
-      <c r="Y19" s="20">
+        <v>#VALUE!</v>
+      </c>
+      <c r="Y19" s="20" t="e">
         <f>ABS(_xll.RtGet(SourceAlias,$U19,ASK)-W19)</f>
-        <v>1.5681900222830336E-14</v>
+        <v>#VALUE!</v>
       </c>
       <c r="Z19" s="2"/>
       <c r="AA19" s="2"/>
@@ -8111,13 +8123,13 @@
         <f t="shared" si="5"/>
         <v>0.17000000002759802</v>
       </c>
-      <c r="X20" s="20">
+      <c r="X20" s="20" t="e">
         <f>ABS(_xll.RtGet(SourceAlias,$U20,BID)-V20)</f>
-        <v>2.7598007212858988E-11</v>
-      </c>
-      <c r="Y20" s="20">
+        <v>#VALUE!</v>
+      </c>
+      <c r="Y20" s="20" t="e">
         <f>ABS(_xll.RtGet(SourceAlias,$U20,ASK)-W20)</f>
-        <v>2.7598007212858988E-11</v>
+        <v>#VALUE!</v>
       </c>
       <c r="Z20" s="2"/>
       <c r="AA20" s="2"/>
@@ -8197,13 +8209,13 @@
         <f t="shared" si="5"/>
         <v>0.16499999999996096</v>
       </c>
-      <c r="X21" s="20">
+      <c r="X21" s="20" t="e">
         <f>ABS(_xll.RtGet(SourceAlias,$U21,BID)-V21)</f>
-        <v>3.9052094891189881E-14</v>
-      </c>
-      <c r="Y21" s="20">
+        <v>#VALUE!</v>
+      </c>
+      <c r="Y21" s="20" t="e">
         <f>ABS(_xll.RtGet(SourceAlias,$U21,ASK)-W21)</f>
-        <v>3.9052094891189881E-14</v>
+        <v>#VALUE!</v>
       </c>
       <c r="Z21" s="2"/>
       <c r="AA21" s="2"/>
@@ -8267,13 +8279,13 @@
         <f t="shared" si="3"/>
         <v>5.6712328814273842E-2</v>
       </c>
-      <c r="J22" s="20">
+      <c r="J22" s="20" t="e">
         <f>ABS(_xll.RtGet(SourceAlias,$G22,BID)-H22)</f>
-        <v>1.8572615667622472E-10</v>
-      </c>
-      <c r="K22" s="20">
+        <v>#VALUE!</v>
+      </c>
+      <c r="K22" s="20" t="e">
         <f>ABS(_xll.RtGet(SourceAlias,$G22,ASK)-I22)</f>
-        <v>1.8572615667622472E-10</v>
+        <v>#VALUE!</v>
       </c>
       <c r="L22" s="68" t="s">
         <v>120</v>
@@ -8293,13 +8305,13 @@
         <f t="shared" si="4"/>
         <v>0.1150000000000287</v>
       </c>
-      <c r="Q22" s="20">
+      <c r="Q22" s="20" t="e">
         <f>ABS(_xll.RtGet(SourceAlias,$N22,BID)-O22)</f>
-        <v>2.8699265186560297E-14</v>
-      </c>
-      <c r="R22" s="20">
+        <v>#VALUE!</v>
+      </c>
+      <c r="R22" s="20" t="e">
         <f>ABS(_xll.RtGet(SourceAlias,$N22,ASK)-P22)</f>
-        <v>2.8699265186560297E-14</v>
+        <v>#VALUE!</v>
       </c>
       <c r="S22" s="68" t="s">
         <v>120</v>
@@ -8319,13 +8331,13 @@
         <f t="shared" si="5"/>
         <v>0.16499999992872999</v>
       </c>
-      <c r="X22" s="20">
+      <c r="X22" s="20" t="e">
         <f>ABS(_xll.RtGet(SourceAlias,$U22,BID)-V22)</f>
-        <v>7.1270017665270302E-11</v>
-      </c>
-      <c r="Y22" s="20">
+        <v>#VALUE!</v>
+      </c>
+      <c r="Y22" s="20" t="e">
         <f>ABS(_xll.RtGet(SourceAlias,$U22,ASK)-W22)</f>
-        <v>7.1270017665270302E-11</v>
+        <v>#VALUE!</v>
       </c>
       <c r="Z22" s="2"/>
       <c r="AA22" s="2"/>
@@ -8396,13 +8408,13 @@
         <f t="shared" si="4"/>
         <v>0.11000000000054685</v>
       </c>
-      <c r="Q23" s="20">
+      <c r="Q23" s="20" t="e">
         <f>ABS(_xll.RtGet(SourceAlias,$N23,BID)-O23)</f>
-        <v>5.4685422856692867E-13</v>
-      </c>
-      <c r="R23" s="20">
+        <v>#VALUE!</v>
+      </c>
+      <c r="R23" s="20" t="e">
         <f>ABS(_xll.RtGet(SourceAlias,$N23,ASK)-P23)</f>
-        <v>5.4685422856692867E-13</v>
+        <v>#VALUE!</v>
       </c>
       <c r="S23" s="68" t="s">
         <v>120</v>
@@ -8475,13 +8487,13 @@
         <f t="shared" si="3"/>
         <v>5.6712328798361522E-2</v>
       </c>
-      <c r="J24" s="20">
+      <c r="J24" s="20" t="e">
         <f>ABS(_xll.RtGet(SourceAlias,$G24,BID)-H24)</f>
-        <v>2.016384767489221E-10</v>
-      </c>
-      <c r="K24" s="20">
+        <v>#VALUE!</v>
+      </c>
+      <c r="K24" s="20" t="e">
         <f>ABS(_xll.RtGet(SourceAlias,$G24,ASK)-I24)</f>
-        <v>2.016384767489221E-10</v>
+        <v>#VALUE!</v>
       </c>
       <c r="L24" s="68" t="s">
         <v>120</v>
@@ -8495,19 +8507,19 @@
       </c>
       <c r="O24" s="20">
         <f>'3M Pricing'!I24*100</f>
-        <v>0.12124248216521501</v>
+        <v>0.12125099315833315</v>
       </c>
       <c r="P24" s="20">
         <f t="shared" si="4"/>
-        <v>0.12124248216521501</v>
-      </c>
-      <c r="Q24" s="20">
+        <v>0.12125099315833315</v>
+      </c>
+      <c r="Q24" s="20" t="e">
         <f>ABS(_xll.RtGet(SourceAlias,$N24,BID)-O24)</f>
-        <v>1.6521500834087988E-10</v>
-      </c>
-      <c r="R24" s="20">
+        <v>#VALUE!</v>
+      </c>
+      <c r="R24" s="20" t="e">
         <f>ABS(_xll.RtGet(SourceAlias,$N24,ASK)-P24)</f>
-        <v>1.6521500834087988E-10</v>
+        <v>#VALUE!</v>
       </c>
       <c r="S24" s="68" t="s">
         <v>120</v>
@@ -8527,13 +8539,13 @@
         <f t="shared" si="5"/>
         <v>0.17000000000000157</v>
       </c>
-      <c r="X24" s="20">
+      <c r="X24" s="20" t="e">
         <f>ABS(_xll.RtGet(SourceAlias,$U24,BID)-V24)</f>
-        <v>1.5543122344752192E-15</v>
-      </c>
-      <c r="Y24" s="20">
+        <v>#VALUE!</v>
+      </c>
+      <c r="Y24" s="20" t="e">
         <f>ABS(_xll.RtGet(SourceAlias,$U24,ASK)-W24)</f>
-        <v>1.5543122344752192E-15</v>
+        <v>#VALUE!</v>
       </c>
       <c r="Z24" s="2"/>
       <c r="AA24" s="2"/>
@@ -8597,13 +8609,13 @@
         <f t="shared" si="3"/>
         <v>5.6712328790572593E-2</v>
       </c>
-      <c r="J25" s="20">
+      <c r="J25" s="20" t="e">
         <f>ABS(_xll.RtGet(SourceAlias,$G25,BID)-H25)</f>
-        <v>2.0942740597273968E-10</v>
-      </c>
-      <c r="K25" s="20">
+        <v>#VALUE!</v>
+      </c>
+      <c r="K25" s="20" t="e">
         <f>ABS(_xll.RtGet(SourceAlias,$G25,ASK)-I25)</f>
-        <v>2.0942740597273968E-10</v>
+        <v>#VALUE!</v>
       </c>
       <c r="L25" s="68" t="s">
         <v>120</v>
@@ -8617,19 +8629,19 @@
       </c>
       <c r="O25" s="20">
         <f>'3M Pricing'!I25*100</f>
-        <v>0.11932841807051461</v>
+        <v>0.11933686762307567</v>
       </c>
       <c r="P25" s="20">
         <f t="shared" si="4"/>
-        <v>0.11932841807051461</v>
-      </c>
-      <c r="Q25" s="20">
+        <v>0.11933686762307567</v>
+      </c>
+      <c r="Q25" s="20" t="e">
         <f>ABS(_xll.RtGet(SourceAlias,$N25,BID)-O25)</f>
-        <v>7.0514608041527538E-11</v>
-      </c>
-      <c r="R25" s="20">
+        <v>#VALUE!</v>
+      </c>
+      <c r="R25" s="20" t="e">
         <f>ABS(_xll.RtGet(SourceAlias,$N25,ASK)-P25)</f>
-        <v>7.0514608041527538E-11</v>
+        <v>#VALUE!</v>
       </c>
       <c r="S25" s="68" t="s">
         <v>120</v>
@@ -8649,13 +8661,13 @@
         <f t="shared" si="5"/>
         <v>0.16750000000297641</v>
       </c>
-      <c r="X25" s="20">
+      <c r="X25" s="20" t="e">
         <f>ABS(_xll.RtGet(SourceAlias,$U25,BID)-V25)</f>
-        <v>2.9763969067175822E-12</v>
-      </c>
-      <c r="Y25" s="20">
+        <v>#VALUE!</v>
+      </c>
+      <c r="Y25" s="20" t="e">
         <f>ABS(_xll.RtGet(SourceAlias,$U25,ASK)-W25)</f>
-        <v>2.9763969067175822E-12</v>
+        <v>#VALUE!</v>
       </c>
       <c r="Z25" s="2"/>
       <c r="AA25" s="2"/>
@@ -8719,13 +8731,13 @@
         <f t="shared" si="3"/>
         <v>6.1643835632118088E-2</v>
       </c>
-      <c r="J26" s="20">
+      <c r="J26" s="20" t="e">
         <f>ABS(_xll.RtGet(SourceAlias,$G26,BID)-H26)</f>
-        <v>3.6788191243308788E-10</v>
-      </c>
-      <c r="K26" s="20">
+        <v>#VALUE!</v>
+      </c>
+      <c r="K26" s="20" t="e">
         <f>ABS(_xll.RtGet(SourceAlias,$G26,ASK)-I26)</f>
-        <v>3.6788191243308788E-10</v>
+        <v>#VALUE!</v>
       </c>
       <c r="L26" s="68" t="s">
         <v>120</v>
@@ -8739,19 +8751,19 @@
       </c>
       <c r="O26" s="20">
         <f>'3M Pricing'!I26*100</f>
-        <v>0.11672265517532168</v>
+        <v>0.11673176088297291</v>
       </c>
       <c r="P26" s="20">
         <f t="shared" si="4"/>
-        <v>0.11672265517532168</v>
-      </c>
-      <c r="Q26" s="20">
+        <v>0.11673176088297291</v>
+      </c>
+      <c r="Q26" s="20" t="e">
         <f>ABS(_xll.RtGet(SourceAlias,$N26,BID)-O26)</f>
-        <v>1.7532168772316226E-10</v>
-      </c>
-      <c r="R26" s="20">
+        <v>#VALUE!</v>
+      </c>
+      <c r="R26" s="20" t="e">
         <f>ABS(_xll.RtGet(SourceAlias,$N26,ASK)-P26)</f>
-        <v>1.7532168772316226E-10</v>
+        <v>#VALUE!</v>
       </c>
       <c r="S26" s="68" t="s">
         <v>120</v>
@@ -8771,13 +8783,13 @@
         <f t="shared" si="5"/>
         <v>0.17249999999618756</v>
       </c>
-      <c r="X26" s="20">
+      <c r="X26" s="20" t="e">
         <f>ABS(_xll.RtGet(SourceAlias,$U26,BID)-V26)</f>
-        <v>3.8124225998359407E-12</v>
-      </c>
-      <c r="Y26" s="20">
+        <v>#VALUE!</v>
+      </c>
+      <c r="Y26" s="20" t="e">
         <f>ABS(_xll.RtGet(SourceAlias,$U26,ASK)-W26)</f>
-        <v>3.8124225998359407E-12</v>
+        <v>#VALUE!</v>
       </c>
       <c r="Z26" s="2"/>
       <c r="AA26" s="2"/>
@@ -8841,13 +8853,13 @@
         <f t="shared" si="3"/>
         <v>6.9041095902194496E-2</v>
       </c>
-      <c r="J27" s="20">
+      <c r="J27" s="20" t="e">
         <f>ABS(_xll.RtGet(SourceAlias,$G27,BID)-H27)</f>
-        <v>9.7805499810199592E-11</v>
-      </c>
-      <c r="K27" s="20">
+        <v>#VALUE!</v>
+      </c>
+      <c r="K27" s="20" t="e">
         <f>ABS(_xll.RtGet(SourceAlias,$G27,ASK)-I27)</f>
-        <v>9.7805499810199592E-11</v>
+        <v>#VALUE!</v>
       </c>
       <c r="L27" s="68" t="s">
         <v>120</v>
@@ -8861,19 +8873,19 @@
       </c>
       <c r="O27" s="20">
         <f>'3M Pricing'!I27*100</f>
-        <v>0.13661405619209993</v>
+        <v>0.13662627621866699</v>
       </c>
       <c r="P27" s="20">
         <f t="shared" si="4"/>
-        <v>0.13661405619209993</v>
-      </c>
-      <c r="Q27" s="20">
+        <v>0.13662627621866699</v>
+      </c>
+      <c r="Q27" s="20" t="e">
         <f>ABS(_xll.RtGet(SourceAlias,$N27,BID)-O27)</f>
-        <v>1.9209991930502213E-10</v>
-      </c>
-      <c r="R27" s="20">
+        <v>#VALUE!</v>
+      </c>
+      <c r="R27" s="20" t="e">
         <f>ABS(_xll.RtGet(SourceAlias,$N27,ASK)-P27)</f>
-        <v>1.9209991930502213E-10</v>
+        <v>#VALUE!</v>
       </c>
       <c r="S27" s="68" t="s">
         <v>120</v>
@@ -8893,13 +8905,13 @@
         <f t="shared" si="5"/>
         <v>0.2000000000159049</v>
       </c>
-      <c r="X27" s="20">
+      <c r="X27" s="20" t="e">
         <f>ABS(_xll.RtGet(SourceAlias,$U27,BID)-V27)</f>
-        <v>1.5904888517326299E-11</v>
-      </c>
-      <c r="Y27" s="20">
+        <v>#VALUE!</v>
+      </c>
+      <c r="Y27" s="20" t="e">
         <f>ABS(_xll.RtGet(SourceAlias,$U27,ASK)-W27)</f>
-        <v>1.5904888517326299E-11</v>
+        <v>#VALUE!</v>
       </c>
       <c r="Z27" s="2"/>
       <c r="AA27" s="2"/>
@@ -8963,13 +8975,13 @@
         <f t="shared" si="3"/>
         <v>9.3698630146423781E-2</v>
       </c>
-      <c r="J28" s="20">
+      <c r="J28" s="20" t="e">
         <f>ABS(_xll.RtGet(SourceAlias,$G28,BID)-H28)</f>
-        <v>1.464237758819209E-10</v>
-      </c>
-      <c r="K28" s="20">
+        <v>#VALUE!</v>
+      </c>
+      <c r="K28" s="20" t="e">
         <f>ABS(_xll.RtGet(SourceAlias,$G28,ASK)-I28)</f>
-        <v>1.464237758819209E-10</v>
+        <v>#VALUE!</v>
       </c>
       <c r="L28" s="68" t="s">
         <v>120</v>
@@ -8983,19 +8995,19 @@
       </c>
       <c r="O28" s="20">
         <f>'3M Pricing'!I28*100</f>
-        <v>0.17392729680225957</v>
+        <v>0.17394889189962787</v>
       </c>
       <c r="P28" s="20">
         <f t="shared" si="4"/>
-        <v>0.17392729680225957</v>
-      </c>
-      <c r="Q28" s="20">
+        <v>0.17394889189962787</v>
+      </c>
+      <c r="Q28" s="20" t="e">
         <f>ABS(_xll.RtGet(SourceAlias,$N28,BID)-O28)</f>
-        <v>1.9774043513720585E-10</v>
-      </c>
-      <c r="R28" s="20">
+        <v>#VALUE!</v>
+      </c>
+      <c r="R28" s="20" t="e">
         <f>ABS(_xll.RtGet(SourceAlias,$N28,ASK)-P28)</f>
-        <v>1.9774043513720585E-10</v>
+        <v>#VALUE!</v>
       </c>
       <c r="S28" s="68" t="s">
         <v>120</v>
@@ -9015,13 +9027,13 @@
         <f t="shared" si="5"/>
         <v>0.25000000000008238</v>
       </c>
-      <c r="X28" s="20">
+      <c r="X28" s="20" t="e">
         <f>ABS(_xll.RtGet(SourceAlias,$U28,BID)-V28)</f>
-        <v>8.2378548427186615E-14</v>
-      </c>
-      <c r="Y28" s="20">
+        <v>#VALUE!</v>
+      </c>
+      <c r="Y28" s="20" t="e">
         <f>ABS(_xll.RtGet(SourceAlias,$U28,ASK)-W28)</f>
-        <v>8.2378548427186615E-14</v>
+        <v>#VALUE!</v>
       </c>
       <c r="Z28" s="2"/>
       <c r="AA28" s="2"/>
@@ -9085,13 +9097,13 @@
         <f t="shared" si="3"/>
         <v>0.13561643836404405</v>
       </c>
-      <c r="J29" s="20">
+      <c r="J29" s="20" t="e">
         <f>ABS(_xll.RtGet(SourceAlias,$G29,BID)-H29)</f>
-        <v>3.6404404490930631E-10</v>
-      </c>
-      <c r="K29" s="20">
+        <v>#VALUE!</v>
+      </c>
+      <c r="K29" s="20" t="e">
         <f>ABS(_xll.RtGet(SourceAlias,$G29,ASK)-I29)</f>
-        <v>3.6404404490930631E-10</v>
+        <v>#VALUE!</v>
       </c>
       <c r="L29" s="68" t="s">
         <v>120</v>
@@ -9105,19 +9117,19 @@
       </c>
       <c r="O29" s="20">
         <f>'3M Pricing'!I29*100</f>
-        <v>0.23629592513786651</v>
+        <v>0.23633893995400981</v>
       </c>
       <c r="P29" s="20">
         <f t="shared" si="4"/>
-        <v>0.23629592513786651</v>
-      </c>
-      <c r="Q29" s="20">
+        <v>0.23633893995400981</v>
+      </c>
+      <c r="Q29" s="20" t="e">
         <f>ABS(_xll.RtGet(SourceAlias,$N29,BID)-O29)</f>
-        <v>1.3786652375280539E-10</v>
-      </c>
-      <c r="R29" s="20">
+        <v>#VALUE!</v>
+      </c>
+      <c r="R29" s="20" t="e">
         <f>ABS(_xll.RtGet(SourceAlias,$N29,ASK)-P29)</f>
-        <v>1.3786652375280539E-10</v>
+        <v>#VALUE!</v>
       </c>
       <c r="S29" s="68" t="s">
         <v>120</v>
@@ -9137,13 +9149,13 @@
         <f t="shared" si="5"/>
         <v>0.32000000000004802</v>
       </c>
-      <c r="X29" s="20">
+      <c r="X29" s="20" t="e">
         <f>ABS(_xll.RtGet(SourceAlias,$U29,BID)-V29)</f>
-        <v>4.801714581503802E-14</v>
-      </c>
-      <c r="Y29" s="20">
+        <v>#VALUE!</v>
+      </c>
+      <c r="Y29" s="20" t="e">
         <f>ABS(_xll.RtGet(SourceAlias,$U29,ASK)-W29)</f>
-        <v>4.801714581503802E-14</v>
+        <v>#VALUE!</v>
       </c>
       <c r="Z29" s="2"/>
       <c r="AA29" s="2"/>
@@ -9207,13 +9219,13 @@
         <f t="shared" si="3"/>
         <v>0.19972602740401738</v>
       </c>
-      <c r="J30" s="20">
+      <c r="J30" s="20" t="e">
         <f>ABS(_xll.RtGet(SourceAlias,$G30,BID)-H30)</f>
-        <v>4.0401737511075453E-10</v>
-      </c>
-      <c r="K30" s="20">
+        <v>#VALUE!</v>
+      </c>
+      <c r="K30" s="20" t="e">
         <f>ABS(_xll.RtGet(SourceAlias,$G30,ASK)-I30)</f>
-        <v>4.0401737511075453E-10</v>
+        <v>#VALUE!</v>
       </c>
       <c r="L30" s="68" t="s">
         <v>120</v>
@@ -9227,19 +9239,19 @@
       </c>
       <c r="O30" s="20">
         <f>'3M Pricing'!I30*100</f>
-        <v>0.31114284046993906</v>
+        <v>0.31122569959889484</v>
       </c>
       <c r="P30" s="20">
         <f t="shared" si="4"/>
-        <v>0.31114284046993906</v>
-      </c>
-      <c r="Q30" s="20">
+        <v>0.31122569959889484</v>
+      </c>
+      <c r="Q30" s="20" t="e">
         <f>ABS(_xll.RtGet(SourceAlias,$N30,BID)-O30)</f>
-        <v>4.6993908764392245E-10</v>
-      </c>
-      <c r="R30" s="20">
+        <v>#VALUE!</v>
+      </c>
+      <c r="R30" s="20" t="e">
         <f>ABS(_xll.RtGet(SourceAlias,$N30,ASK)-P30)</f>
-        <v>4.6993908764392245E-10</v>
+        <v>#VALUE!</v>
       </c>
       <c r="S30" s="68" t="s">
         <v>120</v>
@@ -9259,13 +9271,13 @@
         <f t="shared" si="5"/>
         <v>0.40250000000148872</v>
       </c>
-      <c r="X30" s="20">
+      <c r="X30" s="20" t="e">
         <f>ABS(_xll.RtGet(SourceAlias,$U30,BID)-V30)</f>
-        <v>1.4886980537198724E-12</v>
-      </c>
-      <c r="Y30" s="20">
+        <v>#VALUE!</v>
+      </c>
+      <c r="Y30" s="20" t="e">
         <f>ABS(_xll.RtGet(SourceAlias,$U30,ASK)-W30)</f>
-        <v>1.4886980537198724E-12</v>
+        <v>#VALUE!</v>
       </c>
       <c r="Z30" s="2"/>
       <c r="AA30" s="2"/>
@@ -9329,13 +9341,13 @@
         <f t="shared" si="3"/>
         <v>0.26876712329359459</v>
       </c>
-      <c r="J31" s="20">
+      <c r="J31" s="20" t="e">
         <f>ABS(_xll.RtGet(SourceAlias,$G31,BID)-H31)</f>
-        <v>2.9359459308153646E-10</v>
-      </c>
-      <c r="K31" s="20">
+        <v>#VALUE!</v>
+      </c>
+      <c r="K31" s="20" t="e">
         <f>ABS(_xll.RtGet(SourceAlias,$G31,ASK)-I31)</f>
-        <v>2.9359459308153646E-10</v>
+        <v>#VALUE!</v>
       </c>
       <c r="L31" s="68" t="s">
         <v>120</v>
@@ -9349,19 +9361,19 @@
       </c>
       <c r="O31" s="20">
         <f>'3M Pricing'!I31*100</f>
-        <v>0.39343523714308976</v>
+        <v>0.39357507473958447</v>
       </c>
       <c r="P31" s="20">
         <f t="shared" si="4"/>
-        <v>0.39343523714308976</v>
-      </c>
-      <c r="Q31" s="20">
+        <v>0.39357507473958447</v>
+      </c>
+      <c r="Q31" s="20" t="e">
         <f>ABS(_xll.RtGet(SourceAlias,$N31,BID)-O31)</f>
-        <v>1.4308976226118375E-10</v>
-      </c>
-      <c r="R31" s="20">
+        <v>#VALUE!</v>
+      </c>
+      <c r="R31" s="20" t="e">
         <f>ABS(_xll.RtGet(SourceAlias,$N31,ASK)-P31)</f>
-        <v>1.4308976226118375E-10</v>
+        <v>#VALUE!</v>
       </c>
       <c r="S31" s="68" t="s">
         <v>120</v>
@@ -9381,13 +9393,13 @@
         <f t="shared" si="5"/>
         <v>0.49499999999926036</v>
       </c>
-      <c r="X31" s="20">
+      <c r="X31" s="20" t="e">
         <f>ABS(_xll.RtGet(SourceAlias,$U31,BID)-V31)</f>
-        <v>7.3963057900527929E-13</v>
-      </c>
-      <c r="Y31" s="20">
+        <v>#VALUE!</v>
+      </c>
+      <c r="Y31" s="20" t="e">
         <f>ABS(_xll.RtGet(SourceAlias,$U31,ASK)-W31)</f>
-        <v>7.3963057900527929E-13</v>
+        <v>#VALUE!</v>
       </c>
       <c r="Z31" s="2"/>
       <c r="AA31" s="2"/>
@@ -9445,19 +9457,19 @@
       </c>
       <c r="H32" s="20">
         <f>'ON Pricing'!I32*100</f>
-        <v>0.34027397260802461</v>
+        <v>0.34027397260801989</v>
       </c>
       <c r="I32" s="20">
         <f t="shared" si="3"/>
-        <v>0.34027397260802461</v>
-      </c>
-      <c r="J32" s="20">
+        <v>0.34027397260801989</v>
+      </c>
+      <c r="J32" s="20" t="e">
         <f>ABS(_xll.RtGet(SourceAlias,$G32,BID)-H32)</f>
-        <v>3.91975396585309E-10</v>
-      </c>
-      <c r="K32" s="20">
+        <v>#VALUE!</v>
+      </c>
+      <c r="K32" s="20" t="e">
         <f>ABS(_xll.RtGet(SourceAlias,$G32,ASK)-I32)</f>
-        <v>3.91975396585309E-10</v>
+        <v>#VALUE!</v>
       </c>
       <c r="L32" s="68" t="s">
         <v>120</v>
@@ -9471,19 +9483,19 @@
       </c>
       <c r="O32" s="20">
         <f>'3M Pricing'!I32*100</f>
-        <v>0.47824467639373547</v>
+        <v>0.47845826671993996</v>
       </c>
       <c r="P32" s="20">
         <f t="shared" si="4"/>
-        <v>0.47824467639373547</v>
-      </c>
-      <c r="Q32" s="20">
+        <v>0.47845826671993996</v>
+      </c>
+      <c r="Q32" s="20" t="e">
         <f>ABS(_xll.RtGet(SourceAlias,$N32,BID)-O32)</f>
-        <v>3.9373548865739849E-10</v>
-      </c>
-      <c r="R32" s="20">
+        <v>#VALUE!</v>
+      </c>
+      <c r="R32" s="20" t="e">
         <f>ABS(_xll.RtGet(SourceAlias,$N32,ASK)-P32)</f>
-        <v>3.9373548865739849E-10</v>
+        <v>#VALUE!</v>
       </c>
       <c r="S32" s="68" t="s">
         <v>120</v>
@@ -9503,13 +9515,13 @@
         <f t="shared" si="5"/>
         <v>0.58750000000371438</v>
       </c>
-      <c r="X32" s="20">
+      <c r="X32" s="20" t="e">
         <f>ABS(_xll.RtGet(SourceAlias,$U32,BID)-V32)</f>
-        <v>3.7143621511859237E-12</v>
-      </c>
-      <c r="Y32" s="20">
+        <v>#VALUE!</v>
+      </c>
+      <c r="Y32" s="20" t="e">
         <f>ABS(_xll.RtGet(SourceAlias,$U32,ASK)-W32)</f>
-        <v>3.7143621511859237E-12</v>
+        <v>#VALUE!</v>
       </c>
       <c r="Z32" s="2"/>
       <c r="AA32" s="2"/>
@@ -9567,19 +9579,19 @@
       </c>
       <c r="H33" s="20">
         <f>'ON Pricing'!I33*100</f>
-        <v>0.41424657534723147</v>
+        <v>0.41424657534723347</v>
       </c>
       <c r="I33" s="20">
         <f t="shared" si="3"/>
-        <v>0.41424657534723147</v>
-      </c>
-      <c r="J33" s="20">
+        <v>0.41424657534723347</v>
+      </c>
+      <c r="J33" s="20" t="e">
         <f>ABS(_xll.RtGet(SourceAlias,$G33,BID)-H33)</f>
-        <v>3.472314658026221E-10</v>
-      </c>
-      <c r="K33" s="20">
+        <v>#VALUE!</v>
+      </c>
+      <c r="K33" s="20" t="e">
         <f>ABS(_xll.RtGet(SourceAlias,$G33,ASK)-I33)</f>
-        <v>3.472314658026221E-10</v>
+        <v>#VALUE!</v>
       </c>
       <c r="L33" s="68" t="s">
         <v>120</v>
@@ -9593,19 +9605,19 @@
       </c>
       <c r="O33" s="20">
         <f>'3M Pricing'!I33*100</f>
-        <v>0.56303451531308524</v>
+        <v>0.56333959888462748</v>
       </c>
       <c r="P33" s="20">
         <f t="shared" si="4"/>
-        <v>0.56303451531308524</v>
-      </c>
-      <c r="Q33" s="20">
+        <v>0.56333959888462748</v>
+      </c>
+      <c r="Q33" s="20" t="e">
         <f>ABS(_xll.RtGet(SourceAlias,$N33,BID)-O33)</f>
-        <v>3.1308522441264586E-10</v>
-      </c>
-      <c r="R33" s="20">
+        <v>#VALUE!</v>
+      </c>
+      <c r="R33" s="20" t="e">
         <f>ABS(_xll.RtGet(SourceAlias,$N33,ASK)-P33)</f>
-        <v>3.1308522441264586E-10</v>
+        <v>#VALUE!</v>
       </c>
       <c r="S33" s="68" t="s">
         <v>120</v>
@@ -9625,13 +9637,13 @@
         <f t="shared" si="5"/>
         <v>0.67999999999178695</v>
       </c>
-      <c r="X33" s="20">
+      <c r="X33" s="20" t="e">
         <f>ABS(_xll.RtGet(SourceAlias,$U33,BID)-V33)</f>
-        <v>8.2130968692695205E-12</v>
-      </c>
-      <c r="Y33" s="20">
+        <v>#VALUE!</v>
+      </c>
+      <c r="Y33" s="20" t="e">
         <f>ABS(_xll.RtGet(SourceAlias,$U33,ASK)-W33)</f>
-        <v>8.2130968692695205E-12</v>
+        <v>#VALUE!</v>
       </c>
       <c r="Z33" s="2"/>
       <c r="AA33" s="2"/>
@@ -9689,19 +9701,19 @@
       </c>
       <c r="H34" s="20">
         <f>'ON Pricing'!I34*100</f>
-        <v>0.58191780822135974</v>
+        <v>0.5819178082213563</v>
       </c>
       <c r="I34" s="20">
         <f t="shared" si="3"/>
-        <v>0.58191780822135974</v>
-      </c>
-      <c r="J34" s="20">
+        <v>0.5819178082213563</v>
+      </c>
+      <c r="J34" s="20" t="e">
         <f>ABS(_xll.RtGet(SourceAlias,$G34,BID)-H34)</f>
-        <v>2.2135970834114005E-10</v>
-      </c>
-      <c r="K34" s="20">
+        <v>#VALUE!</v>
+      </c>
+      <c r="K34" s="20" t="e">
         <f>ABS(_xll.RtGet(SourceAlias,$G34,ASK)-I34)</f>
-        <v>2.2135970834114005E-10</v>
+        <v>#VALUE!</v>
       </c>
       <c r="L34" s="68" t="s">
         <v>120</v>
@@ -9715,19 +9727,19 @@
       </c>
       <c r="O34" s="20">
         <f>'3M Pricing'!I34*100</f>
-        <v>0.74009947718326374</v>
+        <v>0.74065918094215777</v>
       </c>
       <c r="P34" s="20">
         <f t="shared" si="4"/>
-        <v>0.74009947718326374</v>
-      </c>
-      <c r="Q34" s="20">
+        <v>0.74065918094215777</v>
+      </c>
+      <c r="Q34" s="20" t="e">
         <f>ABS(_xll.RtGet(SourceAlias,$N34,BID)-O34)</f>
-        <v>1.8326373751875735E-10</v>
-      </c>
-      <c r="R34" s="20">
+        <v>#VALUE!</v>
+      </c>
+      <c r="R34" s="20" t="e">
         <f>ABS(_xll.RtGet(SourceAlias,$N34,ASK)-P34)</f>
-        <v>1.8326373751875735E-10</v>
+        <v>#VALUE!</v>
       </c>
       <c r="S34" s="68" t="s">
         <v>120</v>
@@ -9747,13 +9759,13 @@
         <f t="shared" si="5"/>
         <v>0.86750000000106409</v>
       </c>
-      <c r="X34" s="20">
+      <c r="X34" s="20" t="e">
         <f>ABS(_xll.RtGet(SourceAlias,$U34,BID)-V34)</f>
-        <v>1.06403774680075E-12</v>
-      </c>
-      <c r="Y34" s="20">
+        <v>#VALUE!</v>
+      </c>
+      <c r="Y34" s="20" t="e">
         <f>ABS(_xll.RtGet(SourceAlias,$U34,ASK)-W34)</f>
-        <v>1.06403774680075E-12</v>
+        <v>#VALUE!</v>
       </c>
       <c r="Z34" s="2"/>
       <c r="AA34" s="2"/>
@@ -9811,19 +9823,19 @@
       </c>
       <c r="H35" s="20">
         <f>'ON Pricing'!I35*100</f>
-        <v>0.83342465753044948</v>
+        <v>0.83342465753044703</v>
       </c>
       <c r="I35" s="20">
         <f t="shared" si="3"/>
-        <v>0.83342465753044948</v>
-      </c>
-      <c r="J35" s="20">
+        <v>0.83342465753044703</v>
+      </c>
+      <c r="J35" s="20" t="e">
         <f>ABS(_xll.RtGet(SourceAlias,$G35,BID)-H35)</f>
-        <v>4.6955050958530364E-10</v>
-      </c>
-      <c r="K35" s="20">
+        <v>#VALUE!</v>
+      </c>
+      <c r="K35" s="20" t="e">
         <f>ABS(_xll.RtGet(SourceAlias,$G35,ASK)-I35)</f>
-        <v>4.6955050958530364E-10</v>
+        <v>#VALUE!</v>
       </c>
       <c r="L35" s="68" t="s">
         <v>120</v>
@@ -9837,19 +9849,19 @@
       </c>
       <c r="O35" s="20">
         <f>'3M Pricing'!I35*100</f>
-        <v>0.99441074232184035</v>
+        <v>0.99547808617086264</v>
       </c>
       <c r="P35" s="20">
         <f t="shared" si="4"/>
-        <v>0.99441074232184035</v>
-      </c>
-      <c r="Q35" s="20">
+        <v>0.99547808617086264</v>
+      </c>
+      <c r="Q35" s="20" t="e">
         <f>ABS(_xll.RtGet(SourceAlias,$N35,BID)-O35)</f>
-        <v>3.2184033216253738E-10</v>
-      </c>
-      <c r="R35" s="20">
+        <v>#VALUE!</v>
+      </c>
+      <c r="R35" s="20" t="e">
         <f>ABS(_xll.RtGet(SourceAlias,$N35,ASK)-P35)</f>
-        <v>3.2184033216253738E-10</v>
+        <v>#VALUE!</v>
       </c>
       <c r="S35" s="68" t="s">
         <v>120</v>
@@ -9863,19 +9875,19 @@
       </c>
       <c r="V35" s="20">
         <f>'6M Pricing'!I35*100</f>
-        <v>1.1324999999968648</v>
+        <v>1.1324999999968661</v>
       </c>
       <c r="W35" s="20">
         <f t="shared" si="5"/>
-        <v>1.1324999999968648</v>
-      </c>
-      <c r="X35" s="20">
+        <v>1.1324999999968661</v>
+      </c>
+      <c r="X35" s="20" t="e">
         <f>ABS(_xll.RtGet(SourceAlias,$U35,BID)-V35)</f>
-        <v>3.1352698215414421E-12</v>
-      </c>
-      <c r="Y35" s="20">
+        <v>#VALUE!</v>
+      </c>
+      <c r="Y35" s="20" t="e">
         <f>ABS(_xll.RtGet(SourceAlias,$U35,ASK)-W35)</f>
-        <v>3.1352698215414421E-12</v>
+        <v>#VALUE!</v>
       </c>
       <c r="Z35" s="2"/>
       <c r="AA35" s="2"/>
@@ -9933,19 +9945,19 @@
       </c>
       <c r="H36" s="20">
         <f>'ON Pricing'!I36*100</f>
-        <v>1.1441095890391089</v>
+        <v>1.1441095890391055</v>
       </c>
       <c r="I36" s="20">
         <f t="shared" si="3"/>
-        <v>1.1441095890391089</v>
-      </c>
-      <c r="J36" s="20">
+        <v>1.1441095890391055</v>
+      </c>
+      <c r="J36" s="20" t="e">
         <f>ABS(_xll.RtGet(SourceAlias,$G36,BID)-H36)</f>
-        <v>3.9108938310050689E-11</v>
-      </c>
-      <c r="K36" s="20">
+        <v>#VALUE!</v>
+      </c>
+      <c r="K36" s="20" t="e">
         <f>ABS(_xll.RtGet(SourceAlias,$G36,ASK)-I36)</f>
-        <v>3.9108938310050689E-11</v>
+        <v>#VALUE!</v>
       </c>
       <c r="L36" s="68" t="s">
         <v>120</v>
@@ -9959,19 +9971,19 @@
       </c>
       <c r="O36" s="20">
         <f>'3M Pricing'!I36*100</f>
-        <v>1.313468231642885</v>
+        <v>1.3153866585676162</v>
       </c>
       <c r="P36" s="20">
         <f t="shared" si="4"/>
-        <v>1.313468231642885</v>
-      </c>
-      <c r="Q36" s="20">
+        <v>1.3153866585676162</v>
+      </c>
+      <c r="Q36" s="20" t="e">
         <f>ABS(_xll.RtGet(SourceAlias,$N36,BID)-O36)</f>
-        <v>3.5711500423474263E-10</v>
-      </c>
-      <c r="R36" s="20">
+        <v>#VALUE!</v>
+      </c>
+      <c r="R36" s="20" t="e">
         <f>ABS(_xll.RtGet(SourceAlias,$N36,ASK)-P36)</f>
-        <v>3.5711500423474263E-10</v>
+        <v>#VALUE!</v>
       </c>
       <c r="S36" s="68" t="s">
         <v>120</v>
@@ -9985,19 +9997,19 @@
       </c>
       <c r="V36" s="20">
         <f>'6M Pricing'!I36*100</f>
-        <v>1.4549999999994063</v>
+        <v>1.4549999999994072</v>
       </c>
       <c r="W36" s="20">
         <f t="shared" si="5"/>
-        <v>1.4549999999994063</v>
-      </c>
-      <c r="X36" s="20">
+        <v>1.4549999999994072</v>
+      </c>
+      <c r="X36" s="20" t="e">
         <f>ABS(_xll.RtGet(SourceAlias,$U36,BID)-V36)</f>
-        <v>5.9374727356953372E-13</v>
-      </c>
-      <c r="Y36" s="20">
+        <v>#VALUE!</v>
+      </c>
+      <c r="Y36" s="20" t="e">
         <f>ABS(_xll.RtGet(SourceAlias,$U36,ASK)-W36)</f>
-        <v>5.9374727356953372E-13</v>
+        <v>#VALUE!</v>
       </c>
       <c r="Z36" s="2"/>
       <c r="AA36" s="2"/>
@@ -10055,19 +10067,19 @@
       </c>
       <c r="H37" s="20">
         <f>'ON Pricing'!I37*100</f>
-        <v>1.3093150684934969</v>
+        <v>1.309315068493492</v>
       </c>
       <c r="I37" s="20">
         <f t="shared" si="3"/>
-        <v>1.3093150684934969</v>
-      </c>
-      <c r="J37" s="20">
+        <v>1.309315068493492</v>
+      </c>
+      <c r="J37" s="20" t="e">
         <f>ABS(_xll.RtGet(SourceAlias,$G37,BID)-H37)</f>
-        <v>4.9349679898114118E-10</v>
-      </c>
-      <c r="K37" s="20">
+        <v>#VALUE!</v>
+      </c>
+      <c r="K37" s="20" t="e">
         <f>ABS(_xll.RtGet(SourceAlias,$G37,ASK)-I37)</f>
-        <v>4.9349679898114118E-10</v>
+        <v>#VALUE!</v>
       </c>
       <c r="L37" s="68" t="s">
         <v>120</v>
@@ -10081,19 +10093,19 @@
       </c>
       <c r="O37" s="20">
         <f>'3M Pricing'!I37*100</f>
-        <v>1.4851867667262397</v>
+        <v>1.4876593768483692</v>
       </c>
       <c r="P37" s="20">
         <f t="shared" si="4"/>
-        <v>1.4851867667262397</v>
-      </c>
-      <c r="Q37" s="20">
+        <v>1.4876593768483692</v>
+      </c>
+      <c r="Q37" s="20" t="e">
         <f>ABS(_xll.RtGet(SourceAlias,$N37,BID)-O37)</f>
-        <v>2.7376034772430557E-10</v>
-      </c>
-      <c r="R37" s="20">
+        <v>#VALUE!</v>
+      </c>
+      <c r="R37" s="20" t="e">
         <f>ABS(_xll.RtGet(SourceAlias,$N37,ASK)-P37)</f>
-        <v>2.7376034772430557E-10</v>
+        <v>#VALUE!</v>
       </c>
       <c r="S37" s="68" t="s">
         <v>120</v>
@@ -10107,19 +10119,19 @@
       </c>
       <c r="V37" s="20">
         <f>'6M Pricing'!I37*100</f>
-        <v>1.6275000000002815</v>
+        <v>1.6275000000002835</v>
       </c>
       <c r="W37" s="20">
         <f t="shared" si="5"/>
-        <v>1.6275000000002815</v>
-      </c>
-      <c r="X37" s="20">
+        <v>1.6275000000002835</v>
+      </c>
+      <c r="X37" s="20" t="e">
         <f>ABS(_xll.RtGet(SourceAlias,$U37,BID)-V37)</f>
-        <v>2.815525590449397E-13</v>
-      </c>
-      <c r="Y37" s="20">
+        <v>#VALUE!</v>
+      </c>
+      <c r="Y37" s="20" t="e">
         <f>ABS(_xll.RtGet(SourceAlias,$U37,ASK)-W37)</f>
-        <v>2.815525590449397E-13</v>
+        <v>#VALUE!</v>
       </c>
       <c r="Z37" s="2"/>
       <c r="AA37" s="2"/>
@@ -10177,19 +10189,19 @@
       </c>
       <c r="H38" s="22">
         <f>'ON Pricing'!I38*100</f>
-        <v>1.4104109589077345</v>
+        <v>1.4104109589077283</v>
       </c>
       <c r="I38" s="22">
         <f t="shared" si="3"/>
-        <v>1.4104109589077345</v>
-      </c>
-      <c r="J38" s="22">
+        <v>1.4104109589077283</v>
+      </c>
+      <c r="J38" s="22" t="e">
         <f>ABS(_xll.RtGet(SourceAlias,$G38,BID)-H38)</f>
-        <v>9.2265528550683484E-11</v>
-      </c>
-      <c r="K38" s="22">
+        <v>#VALUE!</v>
+      </c>
+      <c r="K38" s="22" t="e">
         <f>ABS(_xll.RtGet(SourceAlias,$G38,ASK)-I38)</f>
-        <v>9.2265528550683484E-11</v>
+        <v>#VALUE!</v>
       </c>
       <c r="L38" s="68" t="s">
         <v>120</v>
@@ -10203,19 +10215,19 @@
       </c>
       <c r="O38" s="22">
         <f>'3M Pricing'!I38*100</f>
-        <v>1.5824294368256731</v>
+        <v>1.5852621963732778</v>
       </c>
       <c r="P38" s="22">
         <f t="shared" si="4"/>
-        <v>1.5824294368256731</v>
-      </c>
-      <c r="Q38" s="22">
+        <v>1.5852621963732778</v>
+      </c>
+      <c r="Q38" s="22" t="e">
         <f>ABS(_xll.RtGet(SourceAlias,$N38,BID)-O38)</f>
-        <v>1.7432699728203715E-10</v>
-      </c>
-      <c r="R38" s="22">
+        <v>#VALUE!</v>
+      </c>
+      <c r="R38" s="22" t="e">
         <f>ABS(_xll.RtGet(SourceAlias,$N38,ASK)-P38)</f>
-        <v>1.7432699728203715E-10</v>
+        <v>#VALUE!</v>
       </c>
       <c r="S38" s="68" t="s">
         <v>120</v>
@@ -10229,19 +10241,19 @@
       </c>
       <c r="V38" s="22">
         <f>'6M Pricing'!I38*100</f>
-        <v>1.7299999999999958</v>
+        <v>1.7299999999999993</v>
       </c>
       <c r="W38" s="22">
         <f t="shared" si="5"/>
-        <v>1.7299999999999958</v>
-      </c>
-      <c r="X38" s="22">
+        <v>1.7299999999999993</v>
+      </c>
+      <c r="X38" s="22" t="e">
         <f>ABS(_xll.RtGet(SourceAlias,$U38,BID)-V38)</f>
-        <v>4.2188474935755949E-15</v>
-      </c>
-      <c r="Y38" s="22">
+        <v>#VALUE!</v>
+      </c>
+      <c r="Y38" s="22" t="e">
         <f>ABS(_xll.RtGet(SourceAlias,$U38,ASK)-W38)</f>
-        <v>4.2188474935755949E-15</v>
+        <v>#VALUE!</v>
       </c>
       <c r="Z38" s="2"/>
       <c r="AA38" s="2"/>
@@ -13597,9 +13609,11 @@
     <col min="11" max="11" width="15.140625" style="10" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="2.7109375" style="7" hidden="1" customWidth="1" outlineLevel="1"/>
     <col min="13" max="13" width="15.140625" style="7" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="14" max="14" width="2.7109375" style="1" customWidth="1" collapsed="1"/>
-    <col min="15" max="15" width="17.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="16" max="26" width="14.85546875" style="1" customWidth="1"/>
+    <col min="14" max="14" width="2.7109375" style="1" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="15" max="15" width="17.28515625" style="1" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="16" max="16" width="14.85546875" style="1" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="17" max="17" width="2.7109375" style="1" customWidth="1" collapsed="1"/>
+    <col min="18" max="26" width="14.85546875" style="1" customWidth="1"/>
     <col min="27" max="30" width="14.85546875" style="13" customWidth="1"/>
     <col min="31" max="147" width="14.85546875" style="1" customWidth="1"/>
     <col min="148" max="16384" width="2.85546875" style="1"/>
@@ -13776,7 +13790,7 @@
       <c r="L5" s="116"/>
       <c r="M5" s="83" t="str">
         <f>_xll.qlOvernightIndex(,"Tonar",0,Currency,LocalCalendar,"Actual/365 (Fixed)",YieldCurve,,Trigger)</f>
-        <v>obj_00495#0002</v>
+        <v>obj_00488#0001</v>
       </c>
       <c r="N5" s="68"/>
       <c r="O5" s="68"/>
@@ -13875,8 +13889,12 @@
         <v>124</v>
       </c>
       <c r="N7" s="68"/>
-      <c r="O7" s="68"/>
-      <c r="P7" s="2"/>
+      <c r="O7" s="8" t="s">
+        <v>134</v>
+      </c>
+      <c r="P7" s="8" t="s">
+        <v>135</v>
+      </c>
       <c r="Q7" s="2"/>
       <c r="R7" s="2"/>
       <c r="S7" s="2"/>
@@ -13918,12 +13936,16 @@
       <c r="K8" s="66"/>
       <c r="L8" s="116"/>
       <c r="M8" s="37" t="str">
-        <f>_xll.qlMakeOIS(,"1W",OvernightIndex,,"0D","Actual/360",,,Trigger)</f>
-        <v>obj_004bc#0002</v>
+        <f>_xll.qlMakeOIS(,IF(D8="SW","1W",D8),OvernightIndex,,ForwardStart,FixDayCounter,,,Trigger)</f>
+        <v>obj_004a7#0044</v>
       </c>
       <c r="N8" s="68"/>
-      <c r="O8" s="68"/>
-      <c r="P8" s="2"/>
+      <c r="O8" s="23" t="s">
+        <v>136</v>
+      </c>
+      <c r="P8" s="23" t="s">
+        <v>137</v>
+      </c>
       <c r="Q8" s="2"/>
       <c r="R8" s="2"/>
       <c r="S8" s="2"/>
@@ -13965,8 +13987,8 @@
       <c r="K9" s="65"/>
       <c r="L9" s="116"/>
       <c r="M9" s="37" t="str">
-        <f>_xll.qlMakeOIS(,D9,OvernightIndex,,"0D","Actual/360",,,Trigger)</f>
-        <v>obj_004a5#0002</v>
+        <f>_xll.qlMakeOIS(,IF(D9="SW","1W",D9),OvernightIndex,,ForwardStart,FixDayCounter,,,Trigger)</f>
+        <v>obj_0048a#0026</v>
       </c>
       <c r="N9" s="68"/>
       <c r="O9" s="68"/>
@@ -14012,8 +14034,8 @@
       <c r="K10" s="65"/>
       <c r="L10" s="116"/>
       <c r="M10" s="37" t="str">
-        <f>_xll.qlMakeOIS(,D10,OvernightIndex,,"0D","Actual/360",,,Trigger)</f>
-        <v>obj_004a6#0002</v>
+        <f>_xll.qlMakeOIS(,IF(D10="SW","1W",D10),OvernightIndex,,ForwardStart,FixDayCounter,,,Trigger)</f>
+        <v>obj_0048f#0003</v>
       </c>
       <c r="N10" s="68"/>
       <c r="O10" s="68"/>
@@ -14062,8 +14084,8 @@
       </c>
       <c r="L11" s="116"/>
       <c r="M11" s="37" t="str">
-        <f>_xll.qlMakeOIS(,D11,OvernightIndex,,"0D","Actual/360",,,Trigger)</f>
-        <v>obj_004a9#0002</v>
+        <f>_xll.qlMakeOIS(,IF(D11="SW","1W",D11),OvernightIndex,,ForwardStart,FixDayCounter,,,Trigger)</f>
+        <v>obj_00498#0007</v>
       </c>
       <c r="N11" s="68"/>
       <c r="O11" s="68"/>
@@ -14112,8 +14134,8 @@
       </c>
       <c r="L12" s="116"/>
       <c r="M12" s="37" t="str">
-        <f>_xll.qlMakeOIS(,D12,OvernightIndex,,"0D","Actual/360",,,Trigger)</f>
-        <v>obj_004ab#0002</v>
+        <f>_xll.qlMakeOIS(,IF(D12="SW","1W",D12),OvernightIndex,,ForwardStart,FixDayCounter,,,Trigger)</f>
+        <v>obj_004ad#0003</v>
       </c>
       <c r="N12" s="68"/>
       <c r="O12" s="68"/>
@@ -14162,8 +14184,8 @@
       </c>
       <c r="L13" s="116"/>
       <c r="M13" s="37" t="str">
-        <f>_xll.qlMakeOIS(,D13,OvernightIndex,,"0D","Actual/360",,,Trigger)</f>
-        <v>obj_004ba#0002</v>
+        <f>_xll.qlMakeOIS(,IF(D13="SW","1W",D13),OvernightIndex,,ForwardStart,FixDayCounter,,,Trigger)</f>
+        <v>obj_0049c#0003</v>
       </c>
       <c r="N13" s="68"/>
       <c r="O13" s="68"/>
@@ -14212,8 +14234,8 @@
       </c>
       <c r="L14" s="116"/>
       <c r="M14" s="37" t="str">
-        <f>_xll.qlMakeOIS(,D14,OvernightIndex,,"0D","Actual/360",,,Trigger)</f>
-        <v>obj_004b6#0002</v>
+        <f>_xll.qlMakeOIS(,IF(D14="SW","1W",D14),OvernightIndex,,ForwardStart,FixDayCounter,,,Trigger)</f>
+        <v>obj_0049e#0003</v>
       </c>
       <c r="N14" s="68"/>
       <c r="O14" s="68"/>
@@ -14262,8 +14284,8 @@
       </c>
       <c r="L15" s="116"/>
       <c r="M15" s="37" t="str">
-        <f>_xll.qlMakeOIS(,D15,OvernightIndex,,"0D","Actual/360",,,Trigger)</f>
-        <v>obj_004b1#0002</v>
+        <f>_xll.qlMakeOIS(,IF(D15="SW","1W",D15),OvernightIndex,,ForwardStart,FixDayCounter,,,Trigger)</f>
+        <v>obj_004a4#0003</v>
       </c>
       <c r="N15" s="68"/>
       <c r="O15" s="68"/>
@@ -14312,8 +14334,8 @@
       </c>
       <c r="L16" s="116"/>
       <c r="M16" s="37" t="str">
-        <f>_xll.qlMakeOIS(,D16,OvernightIndex,,"0D","Actual/360",,,Trigger)</f>
-        <v>obj_004ad#0002</v>
+        <f>_xll.qlMakeOIS(,IF(D16="SW","1W",D16),OvernightIndex,,ForwardStart,FixDayCounter,,,Trigger)</f>
+        <v>obj_0048b#0003</v>
       </c>
       <c r="N16" s="68"/>
       <c r="O16" s="68"/>
@@ -14356,8 +14378,8 @@
       <c r="K17" s="65"/>
       <c r="L17" s="116"/>
       <c r="M17" s="37" t="str">
-        <f>_xll.qlMakeOIS(,D17,OvernightIndex,,"0D","Actual/360",,,Trigger)</f>
-        <v>obj_004bd#0002</v>
+        <f>_xll.qlMakeOIS(,IF(D17="SW","1W",D17),OvernightIndex,,ForwardStart,FixDayCounter,,,Trigger)</f>
+        <v>obj_0048c#0003</v>
       </c>
       <c r="N17" s="68"/>
       <c r="O17" s="68"/>
@@ -14400,8 +14422,8 @@
       <c r="K18" s="65"/>
       <c r="L18" s="116"/>
       <c r="M18" s="37" t="str">
-        <f>_xll.qlMakeOIS(,D18,OvernightIndex,,"0D","Actual/360",,,Trigger)</f>
-        <v>obj_004b2#0002</v>
+        <f>_xll.qlMakeOIS(,IF(D18="SW","1W",D18),OvernightIndex,,ForwardStart,FixDayCounter,,,Trigger)</f>
+        <v>obj_004a6#0003</v>
       </c>
       <c r="N18" s="68"/>
       <c r="O18" s="68"/>
@@ -14450,8 +14472,8 @@
       </c>
       <c r="L19" s="116"/>
       <c r="M19" s="37" t="str">
-        <f>_xll.qlMakeOIS(,D19,OvernightIndex,,"0D","Actual/360",,,Trigger)</f>
-        <v>obj_004a4#0002</v>
+        <f>_xll.qlMakeOIS(,IF(D19="SW","1W",D19),OvernightIndex,,ForwardStart,FixDayCounter,,,Trigger)</f>
+        <v>obj_004aa#0003</v>
       </c>
       <c r="N19" s="68"/>
       <c r="O19" s="68"/>
@@ -14494,8 +14516,8 @@
       <c r="K20" s="65"/>
       <c r="L20" s="116"/>
       <c r="M20" s="37" t="str">
-        <f>_xll.qlMakeOIS(,D20,OvernightIndex,,"0D","Actual/360",,,Trigger)</f>
-        <v>obj_004a1#0002</v>
+        <f>_xll.qlMakeOIS(,IF(D20="SW","1W",D20),OvernightIndex,,ForwardStart,FixDayCounter,,,Trigger)</f>
+        <v>obj_00497#0003</v>
       </c>
       <c r="N20" s="68"/>
       <c r="O20" s="68"/>
@@ -14538,8 +14560,8 @@
       <c r="K21" s="65"/>
       <c r="L21" s="116"/>
       <c r="M21" s="37" t="str">
-        <f>_xll.qlMakeOIS(,D21,OvernightIndex,,"0D","Actual/360",,,Trigger)</f>
-        <v>obj_004a8#0002</v>
+        <f>_xll.qlMakeOIS(,IF(D21="SW","1W",D21),OvernightIndex,,ForwardStart,FixDayCounter,,,Trigger)</f>
+        <v>obj_00495#0003</v>
       </c>
       <c r="N21" s="68"/>
       <c r="O21" s="68"/>
@@ -14588,8 +14610,8 @@
       </c>
       <c r="L22" s="116"/>
       <c r="M22" s="37" t="str">
-        <f>_xll.qlMakeOIS(,D22,OvernightIndex,,"0D","Actual/360",,,Trigger)</f>
-        <v>obj_004a2#0002</v>
+        <f>_xll.qlMakeOIS(,IF(D22="SW","1W",D22),OvernightIndex,,ForwardStart,FixDayCounter,,,Trigger)</f>
+        <v>obj_0049a#0004</v>
       </c>
       <c r="N22" s="68"/>
       <c r="O22" s="68"/>
@@ -14632,8 +14654,8 @@
       <c r="K23" s="65"/>
       <c r="L23" s="116"/>
       <c r="M23" s="37" t="str">
-        <f>_xll.qlMakeOIS(,D23,OvernightIndex,,"0D","Actual/360",,,Trigger)</f>
-        <v>obj_004af#0002</v>
+        <f>_xll.qlMakeOIS(,IF(D23="SW","1W",D23),OvernightIndex,,ForwardStart,FixDayCounter,,,Trigger)</f>
+        <v>obj_004a0#0004</v>
       </c>
       <c r="N23" s="68"/>
       <c r="O23" s="68"/>
@@ -14682,8 +14704,8 @@
       </c>
       <c r="L24" s="116"/>
       <c r="M24" s="37" t="str">
-        <f>_xll.qlMakeOIS(,D24,OvernightIndex,,"0D","Actual/360",,,Trigger)</f>
-        <v>obj_004b3#0002</v>
+        <f>_xll.qlMakeOIS(,IF(D24="SW","1W",D24),OvernightIndex,,ForwardStart,FixDayCounter,,,Trigger)</f>
+        <v>obj_004ac#0004</v>
       </c>
       <c r="N24" s="68"/>
       <c r="O24" s="68"/>
@@ -14732,8 +14754,8 @@
       </c>
       <c r="L25" s="116"/>
       <c r="M25" s="37" t="str">
-        <f>_xll.qlMakeOIS(,D25,OvernightIndex,,"0D","Actual/360",,,Trigger)</f>
-        <v>obj_004b4#0002</v>
+        <f>_xll.qlMakeOIS(,IF(D25="SW","1W",D25),OvernightIndex,,ForwardStart,FixDayCounter,,,Trigger)</f>
+        <v>obj_004a8#0004</v>
       </c>
       <c r="N25" s="68"/>
       <c r="O25" s="68"/>
@@ -14782,8 +14804,8 @@
       </c>
       <c r="L26" s="116"/>
       <c r="M26" s="37" t="str">
-        <f>_xll.qlMakeOIS(,D26,OvernightIndex,,"0D","Actual/360",,,Trigger)</f>
-        <v>obj_004b5#0002</v>
+        <f>_xll.qlMakeOIS(,IF(D26="SW","1W",D26),OvernightIndex,,ForwardStart,FixDayCounter,,,Trigger)</f>
+        <v>obj_0049d#0016</v>
       </c>
       <c r="N26" s="68"/>
       <c r="O26" s="68"/>
@@ -14832,8 +14854,8 @@
       </c>
       <c r="L27" s="116"/>
       <c r="M27" s="37" t="str">
-        <f>_xll.qlMakeOIS(,D27,OvernightIndex,,"0D","Actual/360",,,Trigger)</f>
-        <v>obj_004aa#0002</v>
+        <f>_xll.qlMakeOIS(,IF(D27="SW","1W",D27),OvernightIndex,,ForwardStart,FixDayCounter,,,Trigger)</f>
+        <v>obj_0049b#0004</v>
       </c>
       <c r="N27" s="68"/>
       <c r="O27" s="68"/>
@@ -14882,8 +14904,8 @@
       </c>
       <c r="L28" s="116"/>
       <c r="M28" s="37" t="str">
-        <f>_xll.qlMakeOIS(,D28,OvernightIndex,,"0D","Actual/360",,,Trigger)</f>
-        <v>obj_004ac#0002</v>
+        <f>_xll.qlMakeOIS(,IF(D28="SW","1W",D28),OvernightIndex,,ForwardStart,FixDayCounter,,,Trigger)</f>
+        <v>obj_004a9#0004</v>
       </c>
       <c r="N28" s="68"/>
       <c r="O28" s="68"/>
@@ -14932,8 +14954,8 @@
       </c>
       <c r="L29" s="116"/>
       <c r="M29" s="37" t="str">
-        <f>_xll.qlMakeOIS(,D29,OvernightIndex,,"0D","Actual/360",,,Trigger)</f>
-        <v>obj_004ae#0002</v>
+        <f>_xll.qlMakeOIS(,IF(D29="SW","1W",D29),OvernightIndex,,ForwardStart,FixDayCounter,,,Trigger)</f>
+        <v>obj_00490#0004</v>
       </c>
       <c r="N29" s="68"/>
       <c r="O29" s="68"/>
@@ -14982,8 +15004,8 @@
       </c>
       <c r="L30" s="116"/>
       <c r="M30" s="37" t="str">
-        <f>_xll.qlMakeOIS(,D30,OvernightIndex,,"0D","Actual/360",,,Trigger)</f>
-        <v>obj_004b0#0002</v>
+        <f>_xll.qlMakeOIS(,IF(D30="SW","1W",D30),OvernightIndex,,ForwardStart,FixDayCounter,,,Trigger)</f>
+        <v>obj_004a2#0004</v>
       </c>
       <c r="N30" s="68"/>
       <c r="O30" s="68"/>
@@ -15032,8 +15054,8 @@
       </c>
       <c r="L31" s="116"/>
       <c r="M31" s="37" t="str">
-        <f>_xll.qlMakeOIS(,D31,OvernightIndex,,"0D","Actual/360",,,Trigger)</f>
-        <v>obj_004b7#0002</v>
+        <f>_xll.qlMakeOIS(,IF(D31="SW","1W",D31),OvernightIndex,,ForwardStart,FixDayCounter,,,Trigger)</f>
+        <v>obj_00493#0004</v>
       </c>
       <c r="N31" s="68"/>
       <c r="O31" s="68"/>
@@ -15070,7 +15092,7 @@
       </c>
       <c r="I32" s="79">
         <f>_xll.qlOvernightIndexedSwapFairRate(M32,InterestRatesTrigger)</f>
-        <v>3.4027397260802464E-3</v>
+        <v>3.4027397260801991E-3</v>
       </c>
       <c r="J32" s="65" t="str">
         <f>Contribution!G32</f>
@@ -15082,8 +15104,8 @@
       </c>
       <c r="L32" s="116"/>
       <c r="M32" s="37" t="str">
-        <f>_xll.qlMakeOIS(,D32,OvernightIndex,,"0D","Actual/360",,,Trigger)</f>
-        <v>obj_004bb#0002</v>
+        <f>_xll.qlMakeOIS(,IF(D32="SW","1W",D32),OvernightIndex,,ForwardStart,FixDayCounter,,,Trigger)</f>
+        <v>obj_004ab#0004</v>
       </c>
       <c r="N32" s="68"/>
       <c r="O32" s="68"/>
@@ -15120,7 +15142,7 @@
       </c>
       <c r="I33" s="79">
         <f>_xll.qlOvernightIndexedSwapFairRate(M33,InterestRatesTrigger)</f>
-        <v>4.1424657534723146E-3</v>
+        <v>4.1424657534723346E-3</v>
       </c>
       <c r="J33" s="65" t="str">
         <f>Contribution!G33</f>
@@ -15132,8 +15154,8 @@
       </c>
       <c r="L33" s="116"/>
       <c r="M33" s="37" t="str">
-        <f>_xll.qlMakeOIS(,D33,OvernightIndex,,"0D","Actual/360",,,Trigger)</f>
-        <v>obj_004b8#0002</v>
+        <f>_xll.qlMakeOIS(,IF(D33="SW","1W",D33),OvernightIndex,,ForwardStart,FixDayCounter,,,Trigger)</f>
+        <v>obj_00496#0004</v>
       </c>
       <c r="N33" s="68"/>
       <c r="O33" s="68"/>
@@ -15170,7 +15192,7 @@
       </c>
       <c r="I34" s="79">
         <f>_xll.qlOvernightIndexedSwapFairRate(M34,InterestRatesTrigger)</f>
-        <v>5.8191780822135974E-3</v>
+        <v>5.8191780822135636E-3</v>
       </c>
       <c r="J34" s="65" t="str">
         <f>Contribution!G34</f>
@@ -15182,8 +15204,8 @@
       </c>
       <c r="L34" s="116"/>
       <c r="M34" s="37" t="str">
-        <f>_xll.qlMakeOIS(,D34,OvernightIndex,,"0D","Actual/360",,,Trigger)</f>
-        <v>obj_004b9#0002</v>
+        <f>_xll.qlMakeOIS(,IF(D34="SW","1W",D34),OvernightIndex,,ForwardStart,FixDayCounter,,,Trigger)</f>
+        <v>obj_00499#0004</v>
       </c>
       <c r="N34" s="68"/>
       <c r="O34" s="68"/>
@@ -15220,7 +15242,7 @@
       </c>
       <c r="I35" s="79">
         <f>_xll.qlOvernightIndexedSwapFairRate(M35,InterestRatesTrigger)</f>
-        <v>8.334246575304495E-3</v>
+        <v>8.3342465753044707E-3</v>
       </c>
       <c r="J35" s="65" t="str">
         <f>Contribution!G35</f>
@@ -15232,8 +15254,8 @@
       </c>
       <c r="L35" s="116"/>
       <c r="M35" s="37" t="str">
-        <f>_xll.qlMakeOIS(,D35,OvernightIndex,,"0D","Actual/360",,,Trigger)</f>
-        <v>obj_004a0#0002</v>
+        <f>_xll.qlMakeOIS(,IF(D35="SW","1W",D35),OvernightIndex,,ForwardStart,FixDayCounter,,,Trigger)</f>
+        <v>obj_004a1#0004</v>
       </c>
       <c r="N35" s="68"/>
       <c r="O35" s="68"/>
@@ -15270,7 +15292,7 @@
       </c>
       <c r="I36" s="79">
         <f>_xll.qlOvernightIndexedSwapFairRate(M36,InterestRatesTrigger)</f>
-        <v>1.1441095890391089E-2</v>
+        <v>1.1441095890391054E-2</v>
       </c>
       <c r="J36" s="65" t="str">
         <f>Contribution!G36</f>
@@ -15282,8 +15304,8 @@
       </c>
       <c r="L36" s="116"/>
       <c r="M36" s="37" t="str">
-        <f>_xll.qlMakeOIS(,D36,OvernightIndex,,"0D","Actual/360",,,Trigger)</f>
-        <v>obj_004a7#0002</v>
+        <f>_xll.qlMakeOIS(,IF(D36="SW","1W",D36),OvernightIndex,,ForwardStart,FixDayCounter,,,Trigger)</f>
+        <v>obj_00492#0004</v>
       </c>
       <c r="N36" s="68"/>
       <c r="O36" s="68"/>
@@ -15320,7 +15342,7 @@
       </c>
       <c r="I37" s="79">
         <f>_xll.qlOvernightIndexedSwapFairRate(M37,InterestRatesTrigger)</f>
-        <v>1.3093150684934968E-2</v>
+        <v>1.3093150684934921E-2</v>
       </c>
       <c r="J37" s="65" t="str">
         <f>Contribution!G37</f>
@@ -15332,8 +15354,8 @@
       </c>
       <c r="L37" s="116"/>
       <c r="M37" s="37" t="str">
-        <f>_xll.qlMakeOIS(,D37,OvernightIndex,,"0D","Actual/360",,,Trigger)</f>
-        <v>obj_0049f#0002</v>
+        <f>_xll.qlMakeOIS(,IF(D37="SW","1W",D37),OvernightIndex,,ForwardStart,FixDayCounter,,,Trigger)</f>
+        <v>obj_0049f#0004</v>
       </c>
       <c r="N37" s="68"/>
       <c r="O37" s="68"/>
@@ -15370,7 +15392,7 @@
       </c>
       <c r="I38" s="79">
         <f>_xll.qlOvernightIndexedSwapFairRate(M38,InterestRatesTrigger)</f>
-        <v>1.4104109589077344E-2</v>
+        <v>1.4104109589077284E-2</v>
       </c>
       <c r="J38" s="67" t="str">
         <f>Contribution!G38</f>
@@ -15382,8 +15404,8 @@
       </c>
       <c r="L38" s="116"/>
       <c r="M38" s="39" t="str">
-        <f>_xll.qlMakeOIS(,D38,OvernightIndex,,"0D","Actual/360",,,Trigger)</f>
-        <v>obj_004a3#0002</v>
+        <f>_xll.qlMakeOIS(,IF(D38="SW","1W",D38),OvernightIndex,,ForwardStart,FixDayCounter,,,Trigger)</f>
+        <v>obj_004ae#0014</v>
       </c>
       <c r="N38" s="68"/>
       <c r="O38" s="68"/>
@@ -17136,6 +17158,11 @@
       <c r="Z100" s="2"/>
     </row>
   </sheetData>
+  <dataValidations count="1">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="P8">
+      <formula1>"Actual/Actual (ISDA),Actual/360,30/360 (Bond Basis),30E/360 (Eurobond Basis),Actual/365 (Fixed),Actual/Actual (ISMA),Actual/Actual (AFB),1/1,30/360 (Italian),Simple"</formula1>
+    </dataValidation>
+  </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <ignoredErrors>
     <ignoredError sqref="I34 I38 I37 I36 I35" evalError="1"/>
@@ -17348,7 +17375,7 @@
       <c r="L5" s="112"/>
       <c r="M5" s="23" t="str">
         <f>_xll.qlInterpolation(,InterpolationType,B7:B13,I7:I13,,Trigger)</f>
-        <v>obj_004d4#0002</v>
+        <v>obj_004d3#0001</v>
       </c>
       <c r="N5" s="112"/>
       <c r="O5" s="112"/>
@@ -17453,7 +17480,7 @@
       <c r="L7" s="112"/>
       <c r="M7" s="35" t="str">
         <f>_xll.qlLibor(,Currency,D7,YieldCurve,,Trigger)</f>
-        <v>obj_004c3#0002</v>
+        <v>obj_004b1#0001</v>
       </c>
       <c r="N7" s="112"/>
       <c r="O7" s="112"/>
@@ -17506,7 +17533,7 @@
       <c r="L8" s="112"/>
       <c r="M8" s="38" t="str">
         <f>_xll.qlLibor(,Currency,D8,YieldCurve,,Trigger)</f>
-        <v>obj_004be#0002</v>
+        <v>obj_004b2#0001</v>
       </c>
       <c r="N8" s="112"/>
       <c r="O8" s="112"/>
@@ -17559,7 +17586,7 @@
       <c r="L9" s="112"/>
       <c r="M9" s="38" t="str">
         <f>_xll.qlLibor(,Currency,D9,YieldCurve,,Trigger)</f>
-        <v>obj_004bf#0002</v>
+        <v>obj_004b3#0001</v>
       </c>
       <c r="N9" s="112"/>
       <c r="O9" s="112"/>
@@ -17612,7 +17639,7 @@
       <c r="L10" s="112"/>
       <c r="M10" s="38" t="str">
         <f>_xll.qlLibor(,Currency,D10,YieldCurve,,Trigger)</f>
-        <v>obj_004c0#0002</v>
+        <v>obj_004b4#0001</v>
       </c>
       <c r="N10" s="112"/>
       <c r="O10" s="112"/>
@@ -17665,7 +17692,7 @@
       <c r="L11" s="112"/>
       <c r="M11" s="38" t="str">
         <f>_xll.qlLibor(,Currency,D11,YieldCurve,,Trigger)</f>
-        <v>obj_004c1#0002</v>
+        <v>obj_004af#0001</v>
       </c>
       <c r="N11" s="112"/>
       <c r="O11" s="112"/>
@@ -17718,7 +17745,7 @@
       <c r="L12" s="112"/>
       <c r="M12" s="38" t="str">
         <f>_xll.qlLibor(,Currency,D12,YieldCurve,,Trigger)</f>
-        <v>obj_004c2#0002</v>
+        <v>obj_004b0#0001</v>
       </c>
       <c r="N12" s="112"/>
       <c r="O12" s="112"/>
@@ -18146,7 +18173,7 @@
       </c>
       <c r="I20" s="79">
         <f>_xll.qlIndexFixing(IborIndex,F20,TRUE,InterestRatesTrigger)</f>
-        <v>1.2538872454491104E-3</v>
+        <v>1.2538872454499889E-3</v>
       </c>
       <c r="J20" s="65"/>
       <c r="K20" s="65"/>
@@ -18195,7 +18222,7 @@
       </c>
       <c r="I21" s="79">
         <f>_xll.qlIndexFixing(IborIndex,F21,TRUE,InterestRatesTrigger)</f>
-        <v>1.1918815758001863E-3</v>
+        <v>1.1918815758010552E-3</v>
       </c>
       <c r="J21" s="65"/>
       <c r="K21" s="65"/>
@@ -18357,7 +18384,7 @@
       </c>
       <c r="I24" s="78">
         <f>_xll.qlIndexFixing(M24,F24,TRUE,InterestRatesTrigger)</f>
-        <v>1.2124248216521501E-3</v>
+        <v>1.2125099315833316E-3</v>
       </c>
       <c r="J24" s="66" t="str">
         <f>Contribution!N24</f>
@@ -18367,11 +18394,11 @@
       <c r="L24" s="112"/>
       <c r="M24" s="38" t="str">
         <f>_xll.qlSwapIndex(,"Libor",D24,SettlementDays,Currency,Calendar,FixedLegTenor,FixedLegBDC,FixedLegDayCounter,IborIndex,"JPYON",,Trigger)</f>
-        <v>obj_00491#0003</v>
+        <v>obj_004cd#0002</v>
       </c>
       <c r="N24" s="112"/>
       <c r="O24" s="38" t="s">
-        <v>27</v>
+        <v>18</v>
       </c>
       <c r="P24" s="38" t="s">
         <v>87</v>
@@ -18413,7 +18440,7 @@
       </c>
       <c r="I25" s="79">
         <f>_xll.qlIndexFixing(M25,F25,TRUE,InterestRatesTrigger)</f>
-        <v>1.1932841807051461E-3</v>
+        <v>1.1933686762307567E-3</v>
       </c>
       <c r="J25" s="65" t="str">
         <f>Contribution!N25</f>
@@ -18423,7 +18450,7 @@
       <c r="L25" s="112"/>
       <c r="M25" s="38" t="str">
         <f>_xll.qlSwapIndex(,"Libor",D25,SettlementDays,Currency,Calendar,FixedLegTenor,FixedLegBDC,FixedLegDayCounter,IborIndex,"JPYON",,Trigger)</f>
-        <v>obj_00486#0003</v>
+        <v>obj_004d2#0002</v>
       </c>
       <c r="N25" s="112"/>
       <c r="O25" s="113"/>
@@ -18463,7 +18490,7 @@
       </c>
       <c r="I26" s="79">
         <f>_xll.qlIndexFixing(M26,F26,TRUE,InterestRatesTrigger)</f>
-        <v>1.1672265517532168E-3</v>
+        <v>1.167317608829729E-3</v>
       </c>
       <c r="J26" s="65" t="str">
         <f>Contribution!N26</f>
@@ -18473,7 +18500,7 @@
       <c r="L26" s="112"/>
       <c r="M26" s="38" t="str">
         <f>_xll.qlSwapIndex(,"Libor",D26,SettlementDays,Currency,Calendar,FixedLegTenor,FixedLegBDC,FixedLegDayCounter,IborIndex,"JPYON",,Trigger)</f>
-        <v>obj_00493#0003</v>
+        <v>obj_004d0#0002</v>
       </c>
       <c r="N26" s="112"/>
       <c r="O26" s="112"/>
@@ -18513,7 +18540,7 @@
       </c>
       <c r="I27" s="79">
         <f>_xll.qlIndexFixing(M27,F27,TRUE,InterestRatesTrigger)</f>
-        <v>1.3661405619209994E-3</v>
+        <v>1.3662627621866699E-3</v>
       </c>
       <c r="J27" s="65" t="str">
         <f>Contribution!N27</f>
@@ -18523,7 +18550,7 @@
       <c r="L27" s="112"/>
       <c r="M27" s="38" t="str">
         <f>_xll.qlSwapIndex(,"Libor",D27,SettlementDays,Currency,Calendar,FixedLegTenor,FixedLegBDC,FixedLegDayCounter,IborIndex,"JPYON",,Trigger)</f>
-        <v>obj_0048b#0003</v>
+        <v>obj_004cf#0002</v>
       </c>
       <c r="N27" s="112"/>
       <c r="O27" s="112"/>
@@ -18563,7 +18590,7 @@
       </c>
       <c r="I28" s="79">
         <f>_xll.qlIndexFixing(M28,F28,TRUE,InterestRatesTrigger)</f>
-        <v>1.7392729680225957E-3</v>
+        <v>1.7394889189962786E-3</v>
       </c>
       <c r="J28" s="65" t="str">
         <f>Contribution!N28</f>
@@ -18573,7 +18600,7 @@
       <c r="L28" s="112"/>
       <c r="M28" s="38" t="str">
         <f>_xll.qlSwapIndex(,"Libor",D28,SettlementDays,Currency,Calendar,FixedLegTenor,FixedLegBDC,FixedLegDayCounter,IborIndex,"JPYON",,Trigger)</f>
-        <v>obj_0048d#0003</v>
+        <v>obj_004ca#0002</v>
       </c>
       <c r="N28" s="112"/>
       <c r="O28" s="112"/>
@@ -18613,7 +18640,7 @@
       </c>
       <c r="I29" s="79">
         <f>_xll.qlIndexFixing(M29,F29,TRUE,InterestRatesTrigger)</f>
-        <v>2.3629592513786653E-3</v>
+        <v>2.3633893995400981E-3</v>
       </c>
       <c r="J29" s="65" t="str">
         <f>Contribution!N29</f>
@@ -18623,7 +18650,7 @@
       <c r="L29" s="112"/>
       <c r="M29" s="38" t="str">
         <f>_xll.qlSwapIndex(,"Libor",D29,SettlementDays,Currency,Calendar,FixedLegTenor,FixedLegBDC,FixedLegDayCounter,IborIndex,"JPYON",,Trigger)</f>
-        <v>obj_00490#0003</v>
+        <v>obj_004c1#0002</v>
       </c>
       <c r="N29" s="112"/>
       <c r="O29" s="112"/>
@@ -18663,7 +18690,7 @@
       </c>
       <c r="I30" s="79">
         <f>_xll.qlIndexFixing(M30,F30,TRUE,InterestRatesTrigger)</f>
-        <v>3.1114284046993906E-3</v>
+        <v>3.1122569959889483E-3</v>
       </c>
       <c r="J30" s="65" t="str">
         <f>Contribution!N30</f>
@@ -18673,7 +18700,7 @@
       <c r="L30" s="112"/>
       <c r="M30" s="38" t="str">
         <f>_xll.qlSwapIndex(,"Libor",D30,SettlementDays,Currency,Calendar,FixedLegTenor,FixedLegBDC,FixedLegDayCounter,IborIndex,"JPYON",,Trigger)</f>
-        <v>obj_0048e#0003</v>
+        <v>obj_004b8#0002</v>
       </c>
       <c r="N30" s="112"/>
       <c r="O30" s="112"/>
@@ -18713,7 +18740,7 @@
       </c>
       <c r="I31" s="79">
         <f>_xll.qlIndexFixing(M31,F31,TRUE,InterestRatesTrigger)</f>
-        <v>3.9343523714308977E-3</v>
+        <v>3.9357507473958449E-3</v>
       </c>
       <c r="J31" s="65" t="str">
         <f>Contribution!N31</f>
@@ -18723,7 +18750,7 @@
       <c r="L31" s="112"/>
       <c r="M31" s="38" t="str">
         <f>_xll.qlSwapIndex(,"Libor",D31,SettlementDays,Currency,Calendar,FixedLegTenor,FixedLegBDC,FixedLegDayCounter,IborIndex,"JPYON",,Trigger)</f>
-        <v>obj_00489#0003</v>
+        <v>obj_004c0#0002</v>
       </c>
       <c r="N31" s="112"/>
       <c r="O31" s="112"/>
@@ -18763,7 +18790,7 @@
       </c>
       <c r="I32" s="79">
         <f>_xll.qlIndexFixing(M32,F32,TRUE,InterestRatesTrigger)</f>
-        <v>4.7824467639373544E-3</v>
+        <v>4.7845826671993998E-3</v>
       </c>
       <c r="J32" s="65" t="str">
         <f>Contribution!N32</f>
@@ -18773,7 +18800,7 @@
       <c r="L32" s="112"/>
       <c r="M32" s="38" t="str">
         <f>_xll.qlSwapIndex(,"Libor",D32,SettlementDays,Currency,Calendar,FixedLegTenor,FixedLegBDC,FixedLegDayCounter,IborIndex,"JPYON",,Trigger)</f>
-        <v>obj_00488#0003</v>
+        <v>obj_004bb#0002</v>
       </c>
       <c r="N32" s="112"/>
       <c r="O32" s="112"/>
@@ -18813,7 +18840,7 @@
       </c>
       <c r="I33" s="79">
         <f>_xll.qlIndexFixing(M33,F33,TRUE,InterestRatesTrigger)</f>
-        <v>5.6303451531308528E-3</v>
+        <v>5.6333959888462751E-3</v>
       </c>
       <c r="J33" s="65" t="str">
         <f>Contribution!N33</f>
@@ -18823,7 +18850,7 @@
       <c r="L33" s="112"/>
       <c r="M33" s="38" t="str">
         <f>_xll.qlSwapIndex(,"Libor",D33,SettlementDays,Currency,Calendar,FixedLegTenor,FixedLegBDC,FixedLegDayCounter,IborIndex,"JPYON",,Trigger)</f>
-        <v>obj_0048c#0003</v>
+        <v>obj_004c7#0002</v>
       </c>
       <c r="N33" s="112"/>
       <c r="O33" s="112"/>
@@ -18863,7 +18890,7 @@
       </c>
       <c r="I34" s="79">
         <f>_xll.qlIndexFixing(M34,F34,TRUE,InterestRatesTrigger)</f>
-        <v>7.400994771832637E-3</v>
+        <v>7.4065918094215781E-3</v>
       </c>
       <c r="J34" s="65" t="str">
         <f>Contribution!N34</f>
@@ -18873,7 +18900,7 @@
       <c r="L34" s="112"/>
       <c r="M34" s="38" t="str">
         <f>_xll.qlSwapIndex(,"Libor",D34,SettlementDays,Currency,Calendar,FixedLegTenor,FixedLegBDC,FixedLegDayCounter,IborIndex,"JPYON",,Trigger)</f>
-        <v>obj_0048f#0003</v>
+        <v>obj_004bc#0002</v>
       </c>
       <c r="N34" s="112"/>
       <c r="O34" s="112"/>
@@ -18913,7 +18940,7 @@
       </c>
       <c r="I35" s="79">
         <f>_xll.qlIndexFixing(M35,F35,TRUE,InterestRatesTrigger)</f>
-        <v>9.9441074232184037E-3</v>
+        <v>9.9547808617086262E-3</v>
       </c>
       <c r="J35" s="65" t="str">
         <f>Contribution!N35</f>
@@ -18923,7 +18950,7 @@
       <c r="L35" s="112"/>
       <c r="M35" s="38" t="str">
         <f>_xll.qlSwapIndex(,"Libor",D35,SettlementDays,Currency,Calendar,FixedLegTenor,FixedLegBDC,FixedLegDayCounter,IborIndex,"JPYON",,Trigger)</f>
-        <v>obj_0048a#0003</v>
+        <v>obj_004c4#0002</v>
       </c>
       <c r="N35" s="112"/>
       <c r="O35" s="112"/>
@@ -18963,7 +18990,7 @@
       </c>
       <c r="I36" s="79">
         <f>_xll.qlIndexFixing(M36,F36,TRUE,InterestRatesTrigger)</f>
-        <v>1.313468231642885E-2</v>
+        <v>1.3153866585676161E-2</v>
       </c>
       <c r="J36" s="65" t="str">
         <f>Contribution!N36</f>
@@ -18973,7 +19000,7 @@
       <c r="L36" s="112"/>
       <c r="M36" s="38" t="str">
         <f>_xll.qlSwapIndex(,"Libor",D36,SettlementDays,Currency,Calendar,FixedLegTenor,FixedLegBDC,FixedLegDayCounter,IborIndex,"JPYON",,Trigger)</f>
-        <v>obj_00494#0003</v>
+        <v>obj_004c8#0002</v>
       </c>
       <c r="N36" s="112"/>
       <c r="O36" s="112"/>
@@ -19013,7 +19040,7 @@
       </c>
       <c r="I37" s="79">
         <f>_xll.qlIndexFixing(M37,F37,TRUE,InterestRatesTrigger)</f>
-        <v>1.4851867667262398E-2</v>
+        <v>1.4876593768483692E-2</v>
       </c>
       <c r="J37" s="65" t="str">
         <f>Contribution!N37</f>
@@ -19023,7 +19050,7 @@
       <c r="L37" s="112"/>
       <c r="M37" s="38" t="str">
         <f>_xll.qlSwapIndex(,"Libor",D37,SettlementDays,Currency,Calendar,FixedLegTenor,FixedLegBDC,FixedLegDayCounter,IborIndex,"JPYON",,Trigger)</f>
-        <v>obj_00492#0003</v>
+        <v>obj_004c6#0002</v>
       </c>
       <c r="N37" s="112"/>
       <c r="O37" s="112"/>
@@ -19063,7 +19090,7 @@
       </c>
       <c r="I38" s="82">
         <f>_xll.qlIndexFixing(M38,F38,TRUE,InterestRatesTrigger)</f>
-        <v>1.582429436825673E-2</v>
+        <v>1.5852621963732778E-2</v>
       </c>
       <c r="J38" s="67" t="str">
         <f>Contribution!N38</f>
@@ -19073,7 +19100,7 @@
       <c r="L38" s="112"/>
       <c r="M38" s="40" t="str">
         <f>_xll.qlSwapIndex(,"Libor",D38,SettlementDays,Currency,Calendar,FixedLegTenor,FixedLegBDC,FixedLegDayCounter,IborIndex,"JPYON",,Trigger)</f>
-        <v>obj_00487#0003</v>
+        <v>obj_004b7#0002</v>
       </c>
       <c r="N38" s="112"/>
       <c r="O38" s="112"/>
@@ -21045,7 +21072,7 @@
       <c r="L5" s="68"/>
       <c r="M5" s="23" t="str">
         <f>_xll.qlInterpolation(,InterpolationType,B7:B16,I7:I16,,Trigger)</f>
-        <v>obj_004d3#0002</v>
+        <v>obj_004d4#0001</v>
       </c>
       <c r="N5" s="4"/>
       <c r="O5" s="112"/>
@@ -21150,7 +21177,7 @@
       <c r="L7" s="68"/>
       <c r="M7" s="35" t="str">
         <f>_xll.qlLibor(,Currency,D7,YieldCurve,,Trigger)</f>
-        <v>obj_00499#0002</v>
+        <v>obj_004a3#0001</v>
       </c>
       <c r="N7" s="4"/>
       <c r="O7" s="112"/>
@@ -21203,7 +21230,7 @@
       <c r="L8" s="68"/>
       <c r="M8" s="38" t="str">
         <f>_xll.qlLibor(,Currency,D8,YieldCurve,,Trigger)</f>
-        <v>obj_0049b#0002</v>
+        <v>obj_00486#0001</v>
       </c>
       <c r="N8" s="4"/>
       <c r="O8" s="112"/>
@@ -21256,7 +21283,7 @@
       <c r="L9" s="68"/>
       <c r="M9" s="38" t="str">
         <f>_xll.qlLibor(,Currency,D9,YieldCurve,,Trigger)</f>
-        <v>obj_00496#0002</v>
+        <v>obj_0048d#0001</v>
       </c>
       <c r="N9" s="4"/>
       <c r="O9" s="112"/>
@@ -21309,7 +21336,7 @@
       <c r="L10" s="68"/>
       <c r="M10" s="38" t="str">
         <f>_xll.qlLibor(,Currency,D10,YieldCurve,,Trigger)</f>
-        <v>obj_0049a#0002</v>
+        <v>obj_004a5#0001</v>
       </c>
       <c r="N10" s="4"/>
       <c r="O10" s="112"/>
@@ -21362,7 +21389,7 @@
       <c r="L11" s="68"/>
       <c r="M11" s="38" t="str">
         <f>_xll.qlLibor(,Currency,D11,YieldCurve,,Trigger)</f>
-        <v>obj_00498#0002</v>
+        <v>obj_00494#0001</v>
       </c>
       <c r="N11" s="4"/>
       <c r="O11" s="112"/>
@@ -21415,7 +21442,7 @@
       <c r="L12" s="68"/>
       <c r="M12" s="38" t="str">
         <f>_xll.qlLibor(,Currency,D12,YieldCurve,,Trigger)</f>
-        <v>obj_0049e#0002</v>
+        <v>obj_0048e#0001</v>
       </c>
       <c r="N12" s="4"/>
       <c r="O12" s="112"/>
@@ -21468,7 +21495,7 @@
       <c r="L13" s="68"/>
       <c r="M13" s="38" t="str">
         <f>_xll.qlLibor(,Currency,D13,YieldCurve,,Trigger)</f>
-        <v>obj_0049d#0002</v>
+        <v>obj_00489#0001</v>
       </c>
       <c r="N13" s="4"/>
       <c r="O13" s="112"/>
@@ -21521,7 +21548,7 @@
       <c r="L14" s="68"/>
       <c r="M14" s="38" t="str">
         <f>_xll.qlLibor(,Currency,D14,YieldCurve,,Trigger)</f>
-        <v>obj_00497#0002</v>
+        <v>obj_00491#0001</v>
       </c>
       <c r="N14" s="4"/>
       <c r="O14" s="112"/>
@@ -21574,7 +21601,7 @@
       <c r="L15" s="68"/>
       <c r="M15" s="38" t="str">
         <f>_xll.qlLibor(,Currency,D15,YieldCurve,,Trigger)</f>
-        <v>obj_0049c#0002</v>
+        <v>obj_00487#0001</v>
       </c>
       <c r="N15" s="4"/>
       <c r="O15" s="112"/>
@@ -22067,7 +22094,7 @@
       <c r="L24" s="68"/>
       <c r="M24" s="97" t="str">
         <f>_xll.qlSwapIndex(,"Libor",D24,SettlementDays,Currency,Calendar,FixedLegTenor,FixedLegBDC,FixedLegDayCounter,IborIndex,"JPYON",,Trigger)</f>
-        <v>obj_004c7#0002</v>
+        <v>obj_004ce#0001</v>
       </c>
       <c r="N24" s="123"/>
       <c r="O24" s="35" t="s">
@@ -22126,7 +22153,7 @@
       <c r="L25" s="68"/>
       <c r="M25" s="64" t="str">
         <f>_xll.qlSwapIndex(,"Libor",D25,SettlementDays,Currency,Calendar,FixedLegTenor,FixedLegBDC,FixedLegDayCounter,IborIndex,"JPYON",,Trigger)</f>
-        <v>obj_004cd#0002</v>
+        <v>obj_004cc#0001</v>
       </c>
       <c r="N25" s="123"/>
       <c r="O25" s="113"/>
@@ -22179,7 +22206,7 @@
       <c r="L26" s="68"/>
       <c r="M26" s="64" t="str">
         <f>_xll.qlSwapIndex(,"Libor",D26,SettlementDays,Currency,Calendar,FixedLegTenor,FixedLegBDC,FixedLegDayCounter,IborIndex,"JPYON",,Trigger)</f>
-        <v>obj_004c8#0002</v>
+        <v>obj_004b9#0001</v>
       </c>
       <c r="N26" s="123"/>
       <c r="O26" s="112"/>
@@ -22232,7 +22259,7 @@
       <c r="L27" s="68"/>
       <c r="M27" s="64" t="str">
         <f>_xll.qlSwapIndex(,"Libor",D27,SettlementDays,Currency,Calendar,FixedLegTenor,FixedLegBDC,FixedLegDayCounter,IborIndex,"JPYON",,Trigger)</f>
-        <v>obj_004c4#0002</v>
+        <v>obj_004d1#0001</v>
       </c>
       <c r="N27" s="123"/>
       <c r="O27" s="112"/>
@@ -22285,7 +22312,7 @@
       <c r="L28" s="68"/>
       <c r="M28" s="64" t="str">
         <f>_xll.qlSwapIndex(,"Libor",D28,SettlementDays,Currency,Calendar,FixedLegTenor,FixedLegBDC,FixedLegDayCounter,IborIndex,"JPYON",,Trigger)</f>
-        <v>obj_004ca#0002</v>
+        <v>obj_004c2#0001</v>
       </c>
       <c r="N28" s="123"/>
       <c r="O28" s="112"/>
@@ -22338,7 +22365,7 @@
       <c r="L29" s="68"/>
       <c r="M29" s="64" t="str">
         <f>_xll.qlSwapIndex(,"Libor",D29,SettlementDays,Currency,Calendar,FixedLegTenor,FixedLegBDC,FixedLegDayCounter,IborIndex,"JPYON",,Trigger)</f>
-        <v>obj_004cc#0002</v>
+        <v>obj_004cb#0001</v>
       </c>
       <c r="N29" s="123"/>
       <c r="O29" s="112"/>
@@ -22391,7 +22418,7 @@
       <c r="L30" s="68"/>
       <c r="M30" s="64" t="str">
         <f>_xll.qlSwapIndex(,"Libor",D30,SettlementDays,Currency,Calendar,FixedLegTenor,FixedLegBDC,FixedLegDayCounter,IborIndex,"JPYON",,Trigger)</f>
-        <v>obj_004c6#0002</v>
+        <v>obj_004bd#0001</v>
       </c>
       <c r="N30" s="123"/>
       <c r="O30" s="112"/>
@@ -22444,7 +22471,7 @@
       <c r="L31" s="68"/>
       <c r="M31" s="64" t="str">
         <f>_xll.qlSwapIndex(,"Libor",D31,SettlementDays,Currency,Calendar,FixedLegTenor,FixedLegBDC,FixedLegDayCounter,IborIndex,"JPYON",,Trigger)</f>
-        <v>obj_004d2#0002</v>
+        <v>obj_004c3#0001</v>
       </c>
       <c r="N31" s="123"/>
       <c r="O31" s="112"/>
@@ -22497,7 +22524,7 @@
       <c r="L32" s="68"/>
       <c r="M32" s="64" t="str">
         <f>_xll.qlSwapIndex(,"Libor",D32,SettlementDays,Currency,Calendar,FixedLegTenor,FixedLegBDC,FixedLegDayCounter,IborIndex,"JPYON",,Trigger)</f>
-        <v>obj_004cf#0002</v>
+        <v>obj_004b6#0001</v>
       </c>
       <c r="N32" s="123"/>
       <c r="O32" s="112"/>
@@ -22550,7 +22577,7 @@
       <c r="L33" s="68"/>
       <c r="M33" s="64" t="str">
         <f>_xll.qlSwapIndex(,"Libor",D33,SettlementDays,Currency,Calendar,FixedLegTenor,FixedLegBDC,FixedLegDayCounter,IborIndex,"JPYON",,Trigger)</f>
-        <v>obj_004cb#0002</v>
+        <v>obj_004c9#0001</v>
       </c>
       <c r="N33" s="123"/>
       <c r="O33" s="112"/>
@@ -22603,7 +22630,7 @@
       <c r="L34" s="68"/>
       <c r="M34" s="64" t="str">
         <f>_xll.qlSwapIndex(,"Libor",D34,SettlementDays,Currency,Calendar,FixedLegTenor,FixedLegBDC,FixedLegDayCounter,IborIndex,"JPYON",,Trigger)</f>
-        <v>obj_004d1#0002</v>
+        <v>obj_004bf#0001</v>
       </c>
       <c r="N34" s="123"/>
       <c r="O34" s="112"/>
@@ -22643,7 +22670,7 @@
       </c>
       <c r="I35" s="79">
         <f>_xll.qlIndexFixing(M35,F35,TRUE,InterestRatesTrigger)</f>
-        <v>1.1324999999968648E-2</v>
+        <v>1.1324999999968662E-2</v>
       </c>
       <c r="J35" s="104" t="str">
         <f>Contribution!U35</f>
@@ -22656,7 +22683,7 @@
       <c r="L35" s="68"/>
       <c r="M35" s="64" t="str">
         <f>_xll.qlSwapIndex(,"Libor",D35,SettlementDays,Currency,Calendar,FixedLegTenor,FixedLegBDC,FixedLegDayCounter,IborIndex,"JPYON",,Trigger)</f>
-        <v>obj_004c5#0002</v>
+        <v>obj_004b5#0001</v>
       </c>
       <c r="N35" s="123"/>
       <c r="O35" s="112"/>
@@ -22696,7 +22723,7 @@
       </c>
       <c r="I36" s="79">
         <f>_xll.qlIndexFixing(M36,F36,TRUE,InterestRatesTrigger)</f>
-        <v>1.4549999999994062E-2</v>
+        <v>1.4549999999994071E-2</v>
       </c>
       <c r="J36" s="104" t="str">
         <f>Contribution!U36</f>
@@ -22709,7 +22736,7 @@
       <c r="L36" s="68"/>
       <c r="M36" s="64" t="str">
         <f>_xll.qlSwapIndex(,"Libor",D36,SettlementDays,Currency,Calendar,FixedLegTenor,FixedLegBDC,FixedLegDayCounter,IborIndex,"JPYON",,Trigger)</f>
-        <v>obj_004c9#0002</v>
+        <v>obj_004be#0001</v>
       </c>
       <c r="N36" s="123"/>
       <c r="O36" s="112"/>
@@ -22749,7 +22776,7 @@
       </c>
       <c r="I37" s="79">
         <f>_xll.qlIndexFixing(M37,F37,TRUE,InterestRatesTrigger)</f>
-        <v>1.6275000000002815E-2</v>
+        <v>1.6275000000002836E-2</v>
       </c>
       <c r="J37" s="104" t="str">
         <f>Contribution!U37</f>
@@ -22762,7 +22789,7 @@
       <c r="L37" s="68"/>
       <c r="M37" s="64" t="str">
         <f>_xll.qlSwapIndex(,"Libor",D37,SettlementDays,Currency,Calendar,FixedLegTenor,FixedLegBDC,FixedLegDayCounter,IborIndex,"JPYON",,Trigger)</f>
-        <v>obj_004ce#0002</v>
+        <v>obj_004c5#0001</v>
       </c>
       <c r="N37" s="123"/>
       <c r="O37" s="112"/>
@@ -22802,7 +22829,7 @@
       </c>
       <c r="I38" s="82">
         <f>_xll.qlIndexFixing(M38,F38,TRUE,InterestRatesTrigger)</f>
-        <v>1.7299999999999958E-2</v>
+        <v>1.7299999999999992E-2</v>
       </c>
       <c r="J38" s="105" t="str">
         <f>Contribution!U38</f>
@@ -22815,7 +22842,7 @@
       <c r="L38" s="68"/>
       <c r="M38" s="111" t="str">
         <f>_xll.qlSwapIndex(,"Libor",D38,SettlementDays,Currency,Calendar,FixedLegTenor,FixedLegBDC,FixedLegDayCounter,IborIndex,"JPYON",,Trigger)</f>
-        <v>obj_004d0#0002</v>
+        <v>obj_004ba#0001</v>
       </c>
       <c r="N38" s="123"/>
       <c r="O38" s="112"/>

</xml_diff>